<commit_message>
EV2, falta ETC EAC TCPI
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/CC2 y CI3 Equipo 01.xlsx
+++ b/Planificación del proyecto/CC2 y CI3 Equipo 01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeDicenTecno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Desktop\New folder (5)\Ecommerce-Sports\Planificación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="277">
   <si>
     <t>Nro Hito</t>
   </si>
@@ -848,6 +848,12 @@
   <si>
     <t>OM</t>
   </si>
+  <si>
+    <t>1 hr</t>
+  </si>
+  <si>
+    <t>3:30 hs</t>
+  </si>
 </sst>
 </file>
 
@@ -855,7 +861,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1150,12 +1156,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1304,25 +1310,25 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1543,7 +1549,7 @@
   </sheetPr>
   <dimension ref="A1:AA112"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -5667,91 +5673,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="77"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="76" t="s">
+      <c r="L1" s="70"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="79" t="s">
+      <c r="O1" s="70"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="77"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="76" t="s">
+      <c r="R1" s="70"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="77"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="79" t="s">
+      <c r="U1" s="70"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="76" t="s">
+      <c r="X1" s="70"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="79" t="s">
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="76" t="s">
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="79" t="s">
+      <c r="AG1" s="70"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="78"/>
+      <c r="AJ1" s="70"/>
+      <c r="AK1" s="71"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -5834,20 +5840,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -35873,6 +35879,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
@@ -35881,16 +35897,6 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -35901,8 +35907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK49"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22:J26"/>
+    <sheetView topLeftCell="E22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35915,91 +35921,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="77"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="76" t="s">
+      <c r="L1" s="70"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="79" t="s">
+      <c r="O1" s="70"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="77"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="76" t="s">
+      <c r="R1" s="70"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="77"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="79" t="s">
+      <c r="U1" s="70"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="76" t="s">
+      <c r="X1" s="70"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="79" t="s">
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="76" t="s">
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="79" t="s">
+      <c r="AG1" s="70"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="78"/>
+      <c r="AJ1" s="70"/>
+      <c r="AK1" s="71"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -36082,20 +36088,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -38573,6 +38579,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -38585,12 +38597,6 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38600,8 +38606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:D40"/>
+    <sheetView tabSelected="1" topLeftCell="D39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -38614,79 +38620,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="77"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="76" t="s">
+      <c r="L1" s="70"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="79" t="s">
+      <c r="O1" s="70"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="77"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="76" t="s">
+      <c r="R1" s="70"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="77"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="79" t="s">
+      <c r="U1" s="70"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="76" t="s">
+      <c r="X1" s="70"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="79" t="s">
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="76" t="s">
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="79" t="s">
+      <c r="AG1" s="70"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="78"/>
+      <c r="AJ1" s="70"/>
+      <c r="AK1" s="71"/>
       <c r="AL1" s="66"/>
       <c r="AM1" s="66"/>
       <c r="AN1" s="66"/>
@@ -38697,16 +38703,16 @@
       <c r="AS1" s="53"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -38797,20 +38803,20 @@
       <c r="AS2" s="53"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -39119,7 +39125,9 @@
       <c r="M7" s="45"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
+      <c r="P7" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -39180,7 +39188,9 @@
       <c r="M8" s="45"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
+      <c r="P8" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
@@ -39371,7 +39381,9 @@
       </c>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
+      <c r="P11" s="12" t="s">
+        <v>275</v>
+      </c>
       <c r="Q11" s="11"/>
       <c r="R11" s="13"/>
       <c r="S11" s="11"/>
@@ -39497,7 +39509,9 @@
       <c r="M13" s="45"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
+      <c r="P13" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="Q13" s="11"/>
       <c r="R13" s="13"/>
       <c r="S13" s="11"/>
@@ -39558,7 +39572,9 @@
       <c r="M14" s="45"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
+      <c r="P14" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
@@ -39812,7 +39828,9 @@
       </c>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
+      <c r="P18" s="12" t="s">
+        <v>275</v>
+      </c>
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
       <c r="S18" s="11"/>
@@ -39873,7 +39891,9 @@
       <c r="M19" s="45"/>
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
+      <c r="P19" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
@@ -39934,7 +39954,9 @@
       <c r="M20" s="45"/>
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
+      <c r="P20" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
@@ -40518,9 +40540,7 @@
       <c r="N29" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="O29" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="11"/>
       <c r="R29" s="11"/>
@@ -40582,7 +40602,7 @@
         <v>108</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="P30" s="12" t="s">
         <v>159</v>
@@ -40647,7 +40667,7 @@
         <v>108</v>
       </c>
       <c r="O31" s="12" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="P31" s="12" t="s">
         <v>156</v>
@@ -40712,7 +40732,7 @@
         <v>108</v>
       </c>
       <c r="O32" s="12" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="P32" s="12" t="s">
         <v>108</v>
@@ -40837,8 +40857,12 @@
       <c r="N34" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
+      <c r="O34" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="P34" s="12" t="s">
+        <v>128</v>
+      </c>
       <c r="Q34" s="11"/>
       <c r="R34" s="11"/>
       <c r="S34" s="11"/>
@@ -40898,8 +40922,12 @@
       <c r="N35" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
+      <c r="O35" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="P35" s="12" t="s">
+        <v>128</v>
+      </c>
       <c r="Q35" s="11"/>
       <c r="R35" s="11"/>
       <c r="S35" s="11"/>
@@ -40959,8 +40987,12 @@
       <c r="N36" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
+      <c r="O36" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="P36" s="12" t="s">
+        <v>128</v>
+      </c>
       <c r="Q36" s="11"/>
       <c r="R36" s="11"/>
       <c r="S36" s="11"/>
@@ -41083,8 +41115,12 @@
       <c r="N38" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="O38" s="12"/>
-      <c r="P38" s="12"/>
+      <c r="O38" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="P38" s="12" t="s">
+        <v>134</v>
+      </c>
       <c r="Q38" s="11"/>
       <c r="R38" s="11"/>
       <c r="S38" s="11"/>
@@ -41144,8 +41180,12 @@
       <c r="N39" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="O39" s="12"/>
-      <c r="P39" s="12"/>
+      <c r="O39" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="P39" s="12" t="s">
+        <v>275</v>
+      </c>
       <c r="Q39" s="11"/>
       <c r="R39" s="11"/>
       <c r="S39" s="11"/>
@@ -41205,8 +41245,12 @@
       <c r="N40" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="O40" s="12"/>
-      <c r="P40" s="12"/>
+      <c r="O40" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="P40" s="12" t="s">
+        <v>275</v>
+      </c>
       <c r="Q40" s="11"/>
       <c r="R40" s="11"/>
       <c r="S40" s="11"/>
@@ -41263,7 +41307,9 @@
         <v>117</v>
       </c>
       <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
+      <c r="P41" s="12" t="s">
+        <v>276</v>
+      </c>
       <c r="Q41" s="11"/>
       <c r="R41" s="11"/>
       <c r="S41" s="11"/>
@@ -41323,8 +41369,12 @@
       <c r="N42" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="O42" s="12"/>
-      <c r="P42" s="12"/>
+      <c r="O42" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="P42" s="12" t="s">
+        <v>116</v>
+      </c>
       <c r="Q42" s="11"/>
       <c r="R42" s="11"/>
       <c r="S42" s="11"/>
@@ -41384,8 +41434,12 @@
       <c r="N43" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="O43" s="12"/>
-      <c r="P43" s="12"/>
+      <c r="O43" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="P43" s="12" t="s">
+        <v>275</v>
+      </c>
       <c r="Q43" s="11"/>
       <c r="R43" s="11"/>
       <c r="S43" s="11"/>
@@ -43623,6 +43677,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -43635,12 +43695,6 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cargadas todas las actividades del proyecto en EV3
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/CC2 y CI3 Equipo 01.xlsx
+++ b/Planificación del proyecto/CC2 y CI3 Equipo 01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeDicenTecno\Desktop\project\Ecommerce-Sports\Planificación del proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeDicenTecno\Desktop\PS\Ecommerce-Sports\Planificación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="CC2" sheetId="1" r:id="rId1"/>
@@ -1309,32 +1309,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1344,19 +1347,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1579,8 +1579,8 @@
   </sheetPr>
   <dimension ref="A1:AA112"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q78" sqref="A78:Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1590,20 +1590,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="67" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="69" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1641,16 +1641,16 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="68"/>
+      <c r="A2" s="70"/>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="2">
         <f t="shared" ref="G2:H2" si="0">H2-7</f>
         <v>44067</v>
@@ -5703,91 +5703,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="79"/>
+      <c r="D1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="77"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="76" t="s">
+      <c r="L1" s="72"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="79" t="s">
+      <c r="O1" s="72"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="77"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="76" t="s">
+      <c r="R1" s="72"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="77"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="79" t="s">
+      <c r="U1" s="72"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="76" t="s">
+      <c r="X1" s="72"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="79" t="s">
+      <c r="AA1" s="72"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="76" t="s">
+      <c r="AD1" s="72"/>
+      <c r="AE1" s="73"/>
+      <c r="AF1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="79" t="s">
+      <c r="AG1" s="72"/>
+      <c r="AH1" s="73"/>
+      <c r="AI1" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="78"/>
+      <c r="AJ1" s="72"/>
+      <c r="AK1" s="73"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -5870,20 +5870,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -35909,6 +35909,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
@@ -35917,16 +35927,6 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -35951,91 +35951,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="79"/>
+      <c r="D1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="77"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="76" t="s">
+      <c r="L1" s="72"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="79" t="s">
+      <c r="O1" s="72"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="77"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="76" t="s">
+      <c r="R1" s="72"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="77"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="79" t="s">
+      <c r="U1" s="72"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="76" t="s">
+      <c r="X1" s="72"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="79" t="s">
+      <c r="AA1" s="72"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="76" t="s">
+      <c r="AD1" s="72"/>
+      <c r="AE1" s="73"/>
+      <c r="AF1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="79" t="s">
+      <c r="AG1" s="72"/>
+      <c r="AH1" s="73"/>
+      <c r="AI1" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="78"/>
+      <c r="AJ1" s="72"/>
+      <c r="AK1" s="73"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -36118,20 +36118,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -38609,6 +38609,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -38621,12 +38627,6 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38636,7 +38636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R64" sqref="R64"/>
     </sheetView>
   </sheetViews>
@@ -38650,79 +38650,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="86"/>
+      <c r="D1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="76" t="s">
+      <c r="L1" s="82"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="81"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="79" t="s">
+      <c r="O1" s="82"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="81"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="76" t="s">
+      <c r="R1" s="82"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="81"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="79" t="s">
+      <c r="U1" s="82"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="76" t="s">
+      <c r="X1" s="82"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="79" t="s">
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="76" t="s">
+      <c r="AD1" s="82"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="81"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="79" t="s">
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="83"/>
+      <c r="AI1" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="81"/>
-      <c r="AK1" s="82"/>
+      <c r="AJ1" s="82"/>
+      <c r="AK1" s="83"/>
       <c r="AL1" s="39"/>
       <c r="AM1" s="66"/>
       <c r="AN1" s="66"/>
@@ -38733,16 +38733,16 @@
       <c r="AS1" s="53"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2" s="83"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -38751,12 +38751,12 @@
         <f>K2+6</f>
         <v>44087</v>
       </c>
-      <c r="N2" s="86">
+      <c r="N2" s="67">
         <f>K2+7</f>
         <v>44088</v>
       </c>
       <c r="O2" s="10"/>
-      <c r="P2" s="86">
+      <c r="P2" s="67">
         <f>N2+6</f>
         <v>44094</v>
       </c>
@@ -38769,12 +38769,12 @@
         <f>Q2+6</f>
         <v>44101</v>
       </c>
-      <c r="T2" s="86">
+      <c r="T2" s="67">
         <f>Q2+7</f>
         <v>44102</v>
       </c>
       <c r="U2" s="10"/>
-      <c r="V2" s="86">
+      <c r="V2" s="67">
         <f>T2+6</f>
         <v>44108</v>
       </c>
@@ -38787,12 +38787,12 @@
         <f>W2+6</f>
         <v>44115</v>
       </c>
-      <c r="Z2" s="86">
+      <c r="Z2" s="67">
         <f>W2+7</f>
         <v>44116</v>
       </c>
       <c r="AA2" s="10"/>
-      <c r="AB2" s="86">
+      <c r="AB2" s="67">
         <f>Z2+6</f>
         <v>44122</v>
       </c>
@@ -38805,12 +38805,12 @@
         <f>AC2+6</f>
         <v>44129</v>
       </c>
-      <c r="AF2" s="86">
+      <c r="AF2" s="67">
         <f>AC2+7</f>
         <v>44130</v>
       </c>
       <c r="AG2" s="10"/>
-      <c r="AH2" s="86">
+      <c r="AH2" s="67">
         <f>AF2+6</f>
         <v>44136</v>
       </c>
@@ -38833,20 +38833,20 @@
       <c r="AS2" s="53"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3" s="87"/>
+      <c r="A3" s="85"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -38970,27 +38970,27 @@
       </c>
       <c r="L4" s="45"/>
       <c r="M4" s="45"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
       <c r="Q4" s="45"/>
       <c r="R4" s="45"/>
       <c r="S4" s="45"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="88"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
       <c r="W4" s="45"/>
       <c r="X4" s="45"/>
       <c r="Y4" s="45"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="68"/>
       <c r="AC4" s="45"/>
       <c r="AD4" s="45"/>
       <c r="AE4" s="45"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
+      <c r="AF4" s="68"/>
+      <c r="AG4" s="68"/>
+      <c r="AH4" s="68"/>
       <c r="AI4" s="45"/>
       <c r="AJ4" s="45"/>
       <c r="AK4" s="45"/>
@@ -39027,27 +39027,27 @@
       <c r="M5" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45"/>
       <c r="S5" s="45"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="88"/>
-      <c r="V5" s="88"/>
+      <c r="T5" s="68"/>
+      <c r="U5" s="68"/>
+      <c r="V5" s="68"/>
       <c r="W5" s="45"/>
       <c r="X5" s="45"/>
       <c r="Y5" s="45"/>
-      <c r="Z5" s="88"/>
-      <c r="AA5" s="88"/>
-      <c r="AB5" s="88"/>
+      <c r="Z5" s="68"/>
+      <c r="AA5" s="68"/>
+      <c r="AB5" s="68"/>
       <c r="AC5" s="45"/>
       <c r="AD5" s="45"/>
       <c r="AE5" s="45"/>
-      <c r="AF5" s="88"/>
-      <c r="AG5" s="88"/>
-      <c r="AH5" s="88"/>
+      <c r="AF5" s="68"/>
+      <c r="AG5" s="68"/>
+      <c r="AH5" s="68"/>
       <c r="AI5" s="45"/>
       <c r="AJ5" s="45"/>
       <c r="AK5" s="45"/>
@@ -39092,27 +39092,27 @@
       <c r="M6" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="88"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
       <c r="Q6" s="45"/>
       <c r="R6" s="45"/>
       <c r="S6" s="45"/>
-      <c r="T6" s="88"/>
-      <c r="U6" s="88"/>
-      <c r="V6" s="88"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="68"/>
       <c r="W6" s="45"/>
       <c r="X6" s="45"/>
       <c r="Y6" s="45"/>
-      <c r="Z6" s="88"/>
-      <c r="AA6" s="88"/>
-      <c r="AB6" s="88"/>
+      <c r="Z6" s="68"/>
+      <c r="AA6" s="68"/>
+      <c r="AB6" s="68"/>
       <c r="AC6" s="45"/>
       <c r="AD6" s="45"/>
       <c r="AE6" s="45"/>
-      <c r="AF6" s="88"/>
-      <c r="AG6" s="88"/>
-      <c r="AH6" s="88"/>
+      <c r="AF6" s="68"/>
+      <c r="AG6" s="68"/>
+      <c r="AH6" s="68"/>
       <c r="AI6" s="45"/>
       <c r="AJ6" s="45"/>
       <c r="AK6" s="45"/>
@@ -39153,31 +39153,31 @@
       </c>
       <c r="L7" s="45"/>
       <c r="M7" s="45"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88" t="s">
+      <c r="N7" s="68"/>
+      <c r="O7" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P7" s="88" t="s">
+      <c r="P7" s="68" t="s">
         <v>108</v>
       </c>
       <c r="Q7" s="45"/>
       <c r="R7" s="45"/>
       <c r="S7" s="45"/>
-      <c r="T7" s="88"/>
-      <c r="U7" s="88"/>
-      <c r="V7" s="88"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="68"/>
       <c r="W7" s="45"/>
       <c r="X7" s="45"/>
       <c r="Y7" s="45"/>
-      <c r="Z7" s="88"/>
-      <c r="AA7" s="88"/>
-      <c r="AB7" s="88"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
       <c r="AC7" s="45"/>
       <c r="AD7" s="45"/>
       <c r="AE7" s="45"/>
-      <c r="AF7" s="88"/>
-      <c r="AG7" s="88"/>
-      <c r="AH7" s="88"/>
+      <c r="AF7" s="68"/>
+      <c r="AG7" s="68"/>
+      <c r="AH7" s="68"/>
       <c r="AI7" s="45"/>
       <c r="AJ7" s="45"/>
       <c r="AK7" s="45"/>
@@ -39218,31 +39218,31 @@
       </c>
       <c r="L8" s="45"/>
       <c r="M8" s="45"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88" t="s">
+      <c r="N8" s="68"/>
+      <c r="O8" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P8" s="88" t="s">
+      <c r="P8" s="68" t="s">
         <v>108</v>
       </c>
       <c r="Q8" s="45"/>
       <c r="R8" s="45"/>
       <c r="S8" s="45"/>
-      <c r="T8" s="88"/>
-      <c r="U8" s="88"/>
-      <c r="V8" s="88"/>
+      <c r="T8" s="68"/>
+      <c r="U8" s="68"/>
+      <c r="V8" s="68"/>
       <c r="W8" s="45"/>
       <c r="X8" s="45"/>
       <c r="Y8" s="45"/>
-      <c r="Z8" s="88"/>
-      <c r="AA8" s="88"/>
-      <c r="AB8" s="88"/>
+      <c r="Z8" s="68"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="68"/>
       <c r="AC8" s="45"/>
       <c r="AD8" s="45"/>
       <c r="AE8" s="45"/>
-      <c r="AF8" s="88"/>
-      <c r="AG8" s="88"/>
-      <c r="AH8" s="88"/>
+      <c r="AF8" s="68"/>
+      <c r="AG8" s="68"/>
+      <c r="AH8" s="68"/>
       <c r="AI8" s="45"/>
       <c r="AJ8" s="45"/>
       <c r="AK8" s="45"/>
@@ -39287,27 +39287,27 @@
       <c r="M9" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N9" s="88"/>
-      <c r="O9" s="88"/>
-      <c r="P9" s="88"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
       <c r="Q9" s="45"/>
       <c r="R9" s="45"/>
       <c r="S9" s="45"/>
-      <c r="T9" s="88"/>
-      <c r="U9" s="88"/>
-      <c r="V9" s="88"/>
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="68"/>
       <c r="W9" s="45"/>
       <c r="X9" s="45"/>
       <c r="Y9" s="45"/>
-      <c r="Z9" s="88"/>
-      <c r="AA9" s="88"/>
-      <c r="AB9" s="88"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="68"/>
       <c r="AC9" s="45"/>
       <c r="AD9" s="45"/>
       <c r="AE9" s="45"/>
-      <c r="AF9" s="88"/>
-      <c r="AG9" s="88"/>
-      <c r="AH9" s="88"/>
+      <c r="AF9" s="68"/>
+      <c r="AG9" s="68"/>
+      <c r="AH9" s="68"/>
       <c r="AI9" s="45"/>
       <c r="AJ9" s="45"/>
       <c r="AK9" s="45"/>
@@ -39352,27 +39352,27 @@
       <c r="M10" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-      <c r="P10" s="88"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
       <c r="Q10" s="45"/>
       <c r="R10" s="45"/>
       <c r="S10" s="45"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="68"/>
       <c r="W10" s="45"/>
       <c r="X10" s="45"/>
       <c r="Y10" s="45"/>
-      <c r="Z10" s="88"/>
-      <c r="AA10" s="88"/>
-      <c r="AB10" s="88"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68"/>
       <c r="AC10" s="45"/>
       <c r="AD10" s="45"/>
       <c r="AE10" s="45"/>
-      <c r="AF10" s="88"/>
-      <c r="AG10" s="88"/>
-      <c r="AH10" s="88"/>
+      <c r="AF10" s="68"/>
+      <c r="AG10" s="68"/>
+      <c r="AH10" s="68"/>
       <c r="AI10" s="45"/>
       <c r="AJ10" s="45"/>
       <c r="AK10" s="45"/>
@@ -39413,29 +39413,29 @@
       <c r="M11" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88" t="s">
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68" t="s">
         <v>275</v>
       </c>
       <c r="Q11" s="45"/>
       <c r="R11" s="45"/>
       <c r="S11" s="45"/>
-      <c r="T11" s="88"/>
-      <c r="U11" s="88"/>
-      <c r="V11" s="88"/>
+      <c r="T11" s="68"/>
+      <c r="U11" s="68"/>
+      <c r="V11" s="68"/>
       <c r="W11" s="45"/>
       <c r="X11" s="45"/>
       <c r="Y11" s="45"/>
-      <c r="Z11" s="88"/>
-      <c r="AA11" s="88"/>
-      <c r="AB11" s="88"/>
+      <c r="Z11" s="68"/>
+      <c r="AA11" s="68"/>
+      <c r="AB11" s="68"/>
       <c r="AC11" s="45"/>
       <c r="AD11" s="45"/>
       <c r="AE11" s="45"/>
-      <c r="AF11" s="88"/>
-      <c r="AG11" s="88"/>
-      <c r="AH11" s="88"/>
+      <c r="AF11" s="68"/>
+      <c r="AG11" s="68"/>
+      <c r="AH11" s="68"/>
       <c r="AI11" s="45"/>
       <c r="AJ11" s="45"/>
       <c r="AK11" s="45"/>
@@ -39480,27 +39480,27 @@
       <c r="M12" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N12" s="88"/>
-      <c r="O12" s="88"/>
-      <c r="P12" s="88"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="68"/>
       <c r="Q12" s="45"/>
       <c r="R12" s="45"/>
       <c r="S12" s="45"/>
-      <c r="T12" s="88"/>
-      <c r="U12" s="88"/>
-      <c r="V12" s="88"/>
+      <c r="T12" s="68"/>
+      <c r="U12" s="68"/>
+      <c r="V12" s="68"/>
       <c r="W12" s="45"/>
       <c r="X12" s="45"/>
       <c r="Y12" s="45"/>
-      <c r="Z12" s="88"/>
-      <c r="AA12" s="88"/>
-      <c r="AB12" s="88"/>
+      <c r="Z12" s="68"/>
+      <c r="AA12" s="68"/>
+      <c r="AB12" s="68"/>
       <c r="AC12" s="45"/>
       <c r="AD12" s="45"/>
       <c r="AE12" s="45"/>
-      <c r="AF12" s="88"/>
-      <c r="AG12" s="88"/>
-      <c r="AH12" s="88"/>
+      <c r="AF12" s="68"/>
+      <c r="AG12" s="68"/>
+      <c r="AH12" s="68"/>
       <c r="AI12" s="45"/>
       <c r="AJ12" s="45"/>
       <c r="AK12" s="45"/>
@@ -39541,31 +39541,31 @@
       </c>
       <c r="L13" s="45"/>
       <c r="M13" s="45"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="88" t="s">
+      <c r="N13" s="68"/>
+      <c r="O13" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P13" s="88" t="s">
+      <c r="P13" s="68" t="s">
         <v>108</v>
       </c>
       <c r="Q13" s="45"/>
       <c r="R13" s="45"/>
       <c r="S13" s="45"/>
-      <c r="T13" s="88"/>
-      <c r="U13" s="88"/>
-      <c r="V13" s="88"/>
+      <c r="T13" s="68"/>
+      <c r="U13" s="68"/>
+      <c r="V13" s="68"/>
       <c r="W13" s="45"/>
       <c r="X13" s="45"/>
       <c r="Y13" s="45"/>
-      <c r="Z13" s="88"/>
-      <c r="AA13" s="88"/>
-      <c r="AB13" s="88"/>
+      <c r="Z13" s="68"/>
+      <c r="AA13" s="68"/>
+      <c r="AB13" s="68"/>
       <c r="AC13" s="45"/>
       <c r="AD13" s="45"/>
       <c r="AE13" s="45"/>
-      <c r="AF13" s="88"/>
-      <c r="AG13" s="88"/>
-      <c r="AH13" s="88"/>
+      <c r="AF13" s="68"/>
+      <c r="AG13" s="68"/>
+      <c r="AH13" s="68"/>
       <c r="AI13" s="45"/>
       <c r="AJ13" s="45"/>
       <c r="AK13" s="45"/>
@@ -39606,31 +39606,31 @@
       </c>
       <c r="L14" s="45"/>
       <c r="M14" s="45"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88" t="s">
+      <c r="N14" s="68"/>
+      <c r="O14" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P14" s="88" t="s">
+      <c r="P14" s="68" t="s">
         <v>108</v>
       </c>
       <c r="Q14" s="45"/>
       <c r="R14" s="45"/>
       <c r="S14" s="45"/>
-      <c r="T14" s="88"/>
-      <c r="U14" s="88"/>
-      <c r="V14" s="88"/>
+      <c r="T14" s="68"/>
+      <c r="U14" s="68"/>
+      <c r="V14" s="68"/>
       <c r="W14" s="45"/>
       <c r="X14" s="45"/>
       <c r="Y14" s="45"/>
-      <c r="Z14" s="88"/>
-      <c r="AA14" s="88"/>
-      <c r="AB14" s="88"/>
+      <c r="Z14" s="68"/>
+      <c r="AA14" s="68"/>
+      <c r="AB14" s="68"/>
       <c r="AC14" s="45"/>
       <c r="AD14" s="45"/>
       <c r="AE14" s="45"/>
-      <c r="AF14" s="88"/>
-      <c r="AG14" s="88"/>
-      <c r="AH14" s="88"/>
+      <c r="AF14" s="68"/>
+      <c r="AG14" s="68"/>
+      <c r="AH14" s="68"/>
       <c r="AI14" s="45"/>
       <c r="AJ14" s="45"/>
       <c r="AK14" s="45"/>
@@ -39675,27 +39675,27 @@
       <c r="M15" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N15" s="88"/>
-      <c r="O15" s="88"/>
-      <c r="P15" s="88"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="68"/>
       <c r="Q15" s="45"/>
       <c r="R15" s="45"/>
       <c r="S15" s="45"/>
-      <c r="T15" s="88"/>
-      <c r="U15" s="88"/>
-      <c r="V15" s="88"/>
+      <c r="T15" s="68"/>
+      <c r="U15" s="68"/>
+      <c r="V15" s="68"/>
       <c r="W15" s="45"/>
       <c r="X15" s="45"/>
       <c r="Y15" s="45"/>
-      <c r="Z15" s="88"/>
-      <c r="AA15" s="88"/>
-      <c r="AB15" s="88"/>
+      <c r="Z15" s="68"/>
+      <c r="AA15" s="68"/>
+      <c r="AB15" s="68"/>
       <c r="AC15" s="45"/>
       <c r="AD15" s="45"/>
       <c r="AE15" s="45"/>
-      <c r="AF15" s="88"/>
-      <c r="AG15" s="88"/>
-      <c r="AH15" s="88"/>
+      <c r="AF15" s="68"/>
+      <c r="AG15" s="68"/>
+      <c r="AH15" s="68"/>
       <c r="AI15" s="45"/>
       <c r="AJ15" s="45"/>
       <c r="AK15" s="45"/>
@@ -39740,27 +39740,27 @@
       <c r="M16" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
-      <c r="P16" s="88"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="68"/>
       <c r="Q16" s="45"/>
       <c r="R16" s="45"/>
       <c r="S16" s="45"/>
-      <c r="T16" s="88"/>
-      <c r="U16" s="88"/>
-      <c r="V16" s="88"/>
+      <c r="T16" s="68"/>
+      <c r="U16" s="68"/>
+      <c r="V16" s="68"/>
       <c r="W16" s="45"/>
       <c r="X16" s="45"/>
       <c r="Y16" s="45"/>
-      <c r="Z16" s="88"/>
-      <c r="AA16" s="88"/>
-      <c r="AB16" s="88"/>
+      <c r="Z16" s="68"/>
+      <c r="AA16" s="68"/>
+      <c r="AB16" s="68"/>
       <c r="AC16" s="45"/>
       <c r="AD16" s="45"/>
       <c r="AE16" s="45"/>
-      <c r="AF16" s="88"/>
-      <c r="AG16" s="88"/>
-      <c r="AH16" s="88"/>
+      <c r="AF16" s="68"/>
+      <c r="AG16" s="68"/>
+      <c r="AH16" s="68"/>
       <c r="AI16" s="45"/>
       <c r="AJ16" s="45"/>
       <c r="AK16" s="45"/>
@@ -39799,27 +39799,27 @@
       <c r="M17" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="N17" s="88"/>
-      <c r="O17" s="88"/>
-      <c r="P17" s="88"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="68"/>
       <c r="Q17" s="45"/>
       <c r="R17" s="45"/>
       <c r="S17" s="45"/>
-      <c r="T17" s="88"/>
-      <c r="U17" s="88"/>
-      <c r="V17" s="88"/>
+      <c r="T17" s="68"/>
+      <c r="U17" s="68"/>
+      <c r="V17" s="68"/>
       <c r="W17" s="45"/>
       <c r="X17" s="45"/>
       <c r="Y17" s="45"/>
-      <c r="Z17" s="88"/>
-      <c r="AA17" s="88"/>
-      <c r="AB17" s="88"/>
+      <c r="Z17" s="68"/>
+      <c r="AA17" s="68"/>
+      <c r="AB17" s="68"/>
       <c r="AC17" s="45"/>
       <c r="AD17" s="45"/>
       <c r="AE17" s="45"/>
-      <c r="AF17" s="88"/>
-      <c r="AG17" s="88"/>
-      <c r="AH17" s="88"/>
+      <c r="AF17" s="68"/>
+      <c r="AG17" s="68"/>
+      <c r="AH17" s="68"/>
       <c r="AI17" s="45"/>
       <c r="AJ17" s="45"/>
       <c r="AK17" s="45"/>
@@ -39864,29 +39864,29 @@
       <c r="M18" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="N18" s="88"/>
-      <c r="O18" s="88"/>
-      <c r="P18" s="88" t="s">
+      <c r="N18" s="68"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="68" t="s">
         <v>275</v>
       </c>
       <c r="Q18" s="45"/>
       <c r="R18" s="45"/>
       <c r="S18" s="45"/>
-      <c r="T18" s="88"/>
-      <c r="U18" s="88"/>
-      <c r="V18" s="88"/>
+      <c r="T18" s="68"/>
+      <c r="U18" s="68"/>
+      <c r="V18" s="68"/>
       <c r="W18" s="45"/>
       <c r="X18" s="45"/>
       <c r="Y18" s="45"/>
-      <c r="Z18" s="88"/>
-      <c r="AA18" s="88"/>
-      <c r="AB18" s="88"/>
+      <c r="Z18" s="68"/>
+      <c r="AA18" s="68"/>
+      <c r="AB18" s="68"/>
       <c r="AC18" s="45"/>
       <c r="AD18" s="45"/>
       <c r="AE18" s="45"/>
-      <c r="AF18" s="88"/>
-      <c r="AG18" s="88"/>
-      <c r="AH18" s="88"/>
+      <c r="AF18" s="68"/>
+      <c r="AG18" s="68"/>
+      <c r="AH18" s="68"/>
       <c r="AI18" s="45"/>
       <c r="AJ18" s="45"/>
       <c r="AK18" s="45"/>
@@ -39927,31 +39927,31 @@
       </c>
       <c r="L19" s="45"/>
       <c r="M19" s="45"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="88" t="s">
+      <c r="N19" s="68"/>
+      <c r="O19" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P19" s="88" t="s">
+      <c r="P19" s="68" t="s">
         <v>108</v>
       </c>
       <c r="Q19" s="45"/>
       <c r="R19" s="45"/>
       <c r="S19" s="45"/>
-      <c r="T19" s="88"/>
-      <c r="U19" s="88"/>
-      <c r="V19" s="88"/>
+      <c r="T19" s="68"/>
+      <c r="U19" s="68"/>
+      <c r="V19" s="68"/>
       <c r="W19" s="45"/>
       <c r="X19" s="45"/>
       <c r="Y19" s="45"/>
-      <c r="Z19" s="88"/>
-      <c r="AA19" s="88"/>
-      <c r="AB19" s="88"/>
+      <c r="Z19" s="68"/>
+      <c r="AA19" s="68"/>
+      <c r="AB19" s="68"/>
       <c r="AC19" s="45"/>
       <c r="AD19" s="45"/>
       <c r="AE19" s="45"/>
-      <c r="AF19" s="88"/>
-      <c r="AG19" s="88"/>
-      <c r="AH19" s="88"/>
+      <c r="AF19" s="68"/>
+      <c r="AG19" s="68"/>
+      <c r="AH19" s="68"/>
       <c r="AI19" s="45"/>
       <c r="AJ19" s="45"/>
       <c r="AK19" s="45"/>
@@ -39992,31 +39992,31 @@
       </c>
       <c r="L20" s="45"/>
       <c r="M20" s="45"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88" t="s">
+      <c r="N20" s="68"/>
+      <c r="O20" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P20" s="88" t="s">
+      <c r="P20" s="68" t="s">
         <v>108</v>
       </c>
       <c r="Q20" s="45"/>
       <c r="R20" s="45"/>
       <c r="S20" s="45"/>
-      <c r="T20" s="88"/>
-      <c r="U20" s="88"/>
-      <c r="V20" s="88"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="68"/>
+      <c r="V20" s="68"/>
       <c r="W20" s="45"/>
       <c r="X20" s="45"/>
       <c r="Y20" s="45"/>
-      <c r="Z20" s="88"/>
-      <c r="AA20" s="88"/>
-      <c r="AB20" s="88"/>
+      <c r="Z20" s="68"/>
+      <c r="AA20" s="68"/>
+      <c r="AB20" s="68"/>
       <c r="AC20" s="45"/>
       <c r="AD20" s="45"/>
       <c r="AE20" s="45"/>
-      <c r="AF20" s="88"/>
-      <c r="AG20" s="88"/>
-      <c r="AH20" s="88"/>
+      <c r="AF20" s="68"/>
+      <c r="AG20" s="68"/>
+      <c r="AH20" s="68"/>
       <c r="AI20" s="45"/>
       <c r="AJ20" s="45"/>
       <c r="AK20" s="45"/>
@@ -40061,27 +40061,27 @@
       <c r="M21" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N21" s="88"/>
-      <c r="O21" s="88"/>
-      <c r="P21" s="88"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="68"/>
       <c r="Q21" s="45"/>
       <c r="R21" s="45"/>
       <c r="S21" s="45"/>
-      <c r="T21" s="88"/>
-      <c r="U21" s="88"/>
-      <c r="V21" s="88"/>
+      <c r="T21" s="68"/>
+      <c r="U21" s="68"/>
+      <c r="V21" s="68"/>
       <c r="W21" s="45"/>
       <c r="X21" s="45"/>
       <c r="Y21" s="45"/>
-      <c r="Z21" s="88"/>
-      <c r="AA21" s="88"/>
-      <c r="AB21" s="88"/>
+      <c r="Z21" s="68"/>
+      <c r="AA21" s="68"/>
+      <c r="AB21" s="68"/>
       <c r="AC21" s="45"/>
       <c r="AD21" s="45"/>
       <c r="AE21" s="45"/>
-      <c r="AF21" s="88"/>
-      <c r="AG21" s="88"/>
-      <c r="AH21" s="88"/>
+      <c r="AF21" s="68"/>
+      <c r="AG21" s="68"/>
+      <c r="AH21" s="68"/>
       <c r="AI21" s="45"/>
       <c r="AJ21" s="45"/>
       <c r="AK21" s="45"/>
@@ -40126,27 +40126,27 @@
       <c r="M22" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N22" s="88"/>
-      <c r="O22" s="88"/>
-      <c r="P22" s="88"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="68"/>
+      <c r="P22" s="68"/>
       <c r="Q22" s="45"/>
       <c r="R22" s="45"/>
       <c r="S22" s="45"/>
-      <c r="T22" s="88"/>
-      <c r="U22" s="88"/>
-      <c r="V22" s="88"/>
+      <c r="T22" s="68"/>
+      <c r="U22" s="68"/>
+      <c r="V22" s="68"/>
       <c r="W22" s="45"/>
       <c r="X22" s="45"/>
       <c r="Y22" s="45"/>
-      <c r="Z22" s="88"/>
-      <c r="AA22" s="88"/>
-      <c r="AB22" s="88"/>
+      <c r="Z22" s="68"/>
+      <c r="AA22" s="68"/>
+      <c r="AB22" s="68"/>
       <c r="AC22" s="45"/>
       <c r="AD22" s="45"/>
       <c r="AE22" s="45"/>
-      <c r="AF22" s="88"/>
-      <c r="AG22" s="88"/>
-      <c r="AH22" s="88"/>
+      <c r="AF22" s="68"/>
+      <c r="AG22" s="68"/>
+      <c r="AH22" s="68"/>
       <c r="AI22" s="45"/>
       <c r="AJ22" s="45"/>
       <c r="AK22" s="45"/>
@@ -40187,27 +40187,27 @@
         <v>19</v>
       </c>
       <c r="M23" s="45"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
+      <c r="N23" s="68"/>
+      <c r="O23" s="68"/>
+      <c r="P23" s="68"/>
       <c r="Q23" s="45"/>
       <c r="R23" s="45"/>
       <c r="S23" s="45"/>
-      <c r="T23" s="88"/>
-      <c r="U23" s="88"/>
-      <c r="V23" s="88"/>
+      <c r="T23" s="68"/>
+      <c r="U23" s="68"/>
+      <c r="V23" s="68"/>
       <c r="W23" s="45"/>
       <c r="X23" s="45"/>
       <c r="Y23" s="45"/>
-      <c r="Z23" s="88"/>
-      <c r="AA23" s="88"/>
-      <c r="AB23" s="88"/>
+      <c r="Z23" s="68"/>
+      <c r="AA23" s="68"/>
+      <c r="AB23" s="68"/>
       <c r="AC23" s="45"/>
       <c r="AD23" s="45"/>
       <c r="AE23" s="45"/>
-      <c r="AF23" s="88"/>
-      <c r="AG23" s="88"/>
-      <c r="AH23" s="88"/>
+      <c r="AF23" s="68"/>
+      <c r="AG23" s="68"/>
+      <c r="AH23" s="68"/>
       <c r="AI23" s="45"/>
       <c r="AJ23" s="45"/>
       <c r="AK23" s="45"/>
@@ -40248,27 +40248,27 @@
         <v>19</v>
       </c>
       <c r="M24" s="45"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="88"/>
-      <c r="P24" s="88"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="68"/>
+      <c r="P24" s="68"/>
       <c r="Q24" s="45"/>
       <c r="R24" s="45"/>
       <c r="S24" s="45"/>
-      <c r="T24" s="88"/>
-      <c r="U24" s="88"/>
-      <c r="V24" s="88"/>
+      <c r="T24" s="68"/>
+      <c r="U24" s="68"/>
+      <c r="V24" s="68"/>
       <c r="W24" s="45"/>
       <c r="X24" s="45"/>
       <c r="Y24" s="45"/>
-      <c r="Z24" s="88"/>
-      <c r="AA24" s="88"/>
-      <c r="AB24" s="88"/>
+      <c r="Z24" s="68"/>
+      <c r="AA24" s="68"/>
+      <c r="AB24" s="68"/>
       <c r="AC24" s="45"/>
       <c r="AD24" s="45"/>
       <c r="AE24" s="45"/>
-      <c r="AF24" s="88"/>
-      <c r="AG24" s="88"/>
-      <c r="AH24" s="88"/>
+      <c r="AF24" s="68"/>
+      <c r="AG24" s="68"/>
+      <c r="AH24" s="68"/>
       <c r="AI24" s="45"/>
       <c r="AJ24" s="45"/>
       <c r="AK24" s="45"/>
@@ -40315,27 +40315,27 @@
       <c r="M25" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="N25" s="88"/>
-      <c r="O25" s="88"/>
-      <c r="P25" s="88"/>
+      <c r="N25" s="68"/>
+      <c r="O25" s="68"/>
+      <c r="P25" s="68"/>
       <c r="Q25" s="45"/>
       <c r="R25" s="45"/>
       <c r="S25" s="45"/>
-      <c r="T25" s="88"/>
-      <c r="U25" s="88"/>
-      <c r="V25" s="88"/>
+      <c r="T25" s="68"/>
+      <c r="U25" s="68"/>
+      <c r="V25" s="68"/>
       <c r="W25" s="45"/>
       <c r="X25" s="45"/>
       <c r="Y25" s="45"/>
-      <c r="Z25" s="88"/>
-      <c r="AA25" s="88"/>
-      <c r="AB25" s="88"/>
+      <c r="Z25" s="68"/>
+      <c r="AA25" s="68"/>
+      <c r="AB25" s="68"/>
       <c r="AC25" s="45"/>
       <c r="AD25" s="45"/>
       <c r="AE25" s="45"/>
-      <c r="AF25" s="88"/>
-      <c r="AG25" s="88"/>
-      <c r="AH25" s="88"/>
+      <c r="AF25" s="68"/>
+      <c r="AG25" s="68"/>
+      <c r="AH25" s="68"/>
       <c r="AI25" s="45"/>
       <c r="AJ25" s="45"/>
       <c r="AK25" s="45"/>
@@ -40380,27 +40380,27 @@
       <c r="M26" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
+      <c r="N26" s="68"/>
+      <c r="O26" s="68"/>
+      <c r="P26" s="68"/>
       <c r="Q26" s="45"/>
       <c r="R26" s="45"/>
       <c r="S26" s="45"/>
-      <c r="T26" s="88"/>
-      <c r="U26" s="88"/>
-      <c r="V26" s="88"/>
+      <c r="T26" s="68"/>
+      <c r="U26" s="68"/>
+      <c r="V26" s="68"/>
       <c r="W26" s="45"/>
       <c r="X26" s="45"/>
       <c r="Y26" s="45"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="88"/>
-      <c r="AB26" s="88"/>
+      <c r="Z26" s="68"/>
+      <c r="AA26" s="68"/>
+      <c r="AB26" s="68"/>
       <c r="AC26" s="45"/>
       <c r="AD26" s="45"/>
       <c r="AE26" s="45"/>
-      <c r="AF26" s="88"/>
-      <c r="AG26" s="88"/>
-      <c r="AH26" s="88"/>
+      <c r="AF26" s="68"/>
+      <c r="AG26" s="68"/>
+      <c r="AH26" s="68"/>
       <c r="AI26" s="45"/>
       <c r="AJ26" s="45"/>
       <c r="AK26" s="45"/>
@@ -40449,27 +40449,27 @@
       <c r="M27" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="N27" s="88"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="88"/>
+      <c r="N27" s="68"/>
+      <c r="O27" s="68"/>
+      <c r="P27" s="68"/>
       <c r="Q27" s="45"/>
       <c r="R27" s="45"/>
       <c r="S27" s="45"/>
-      <c r="T27" s="88"/>
-      <c r="U27" s="88"/>
-      <c r="V27" s="88"/>
+      <c r="T27" s="68"/>
+      <c r="U27" s="68"/>
+      <c r="V27" s="68"/>
       <c r="W27" s="45"/>
       <c r="X27" s="45"/>
       <c r="Y27" s="45"/>
-      <c r="Z27" s="88"/>
-      <c r="AA27" s="88"/>
-      <c r="AB27" s="88"/>
+      <c r="Z27" s="68"/>
+      <c r="AA27" s="68"/>
+      <c r="AB27" s="68"/>
       <c r="AC27" s="45"/>
       <c r="AD27" s="45"/>
       <c r="AE27" s="45"/>
-      <c r="AF27" s="88"/>
-      <c r="AG27" s="88"/>
-      <c r="AH27" s="88"/>
+      <c r="AF27" s="68"/>
+      <c r="AG27" s="68"/>
+      <c r="AH27" s="68"/>
       <c r="AI27" s="45"/>
       <c r="AJ27" s="45"/>
       <c r="AK27" s="45"/>
@@ -40518,27 +40518,27 @@
       <c r="M28" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="N28" s="88"/>
-      <c r="O28" s="88"/>
-      <c r="P28" s="88"/>
+      <c r="N28" s="68"/>
+      <c r="O28" s="68"/>
+      <c r="P28" s="68"/>
       <c r="Q28" s="45"/>
       <c r="R28" s="45"/>
       <c r="S28" s="45"/>
-      <c r="T28" s="88"/>
-      <c r="U28" s="88"/>
-      <c r="V28" s="88"/>
+      <c r="T28" s="68"/>
+      <c r="U28" s="68"/>
+      <c r="V28" s="68"/>
       <c r="W28" s="45"/>
       <c r="X28" s="45"/>
       <c r="Y28" s="45"/>
-      <c r="Z28" s="88"/>
-      <c r="AA28" s="88"/>
-      <c r="AB28" s="88"/>
+      <c r="Z28" s="68"/>
+      <c r="AA28" s="68"/>
+      <c r="AB28" s="68"/>
       <c r="AC28" s="45"/>
       <c r="AD28" s="45"/>
       <c r="AE28" s="45"/>
-      <c r="AF28" s="88"/>
-      <c r="AG28" s="88"/>
-      <c r="AH28" s="88"/>
+      <c r="AF28" s="68"/>
+      <c r="AG28" s="68"/>
+      <c r="AH28" s="68"/>
       <c r="AI28" s="45"/>
       <c r="AJ28" s="45"/>
       <c r="AK28" s="45"/>
@@ -40579,29 +40579,29 @@
       <c r="K29" s="45"/>
       <c r="L29" s="45"/>
       <c r="M29" s="45"/>
-      <c r="N29" s="88" t="s">
+      <c r="N29" s="68" t="s">
         <v>153</v>
       </c>
-      <c r="O29" s="88"/>
-      <c r="P29" s="88"/>
+      <c r="O29" s="68"/>
+      <c r="P29" s="68"/>
       <c r="Q29" s="45"/>
       <c r="R29" s="45"/>
       <c r="S29" s="45"/>
-      <c r="T29" s="88"/>
-      <c r="U29" s="88"/>
-      <c r="V29" s="88"/>
+      <c r="T29" s="68"/>
+      <c r="U29" s="68"/>
+      <c r="V29" s="68"/>
       <c r="W29" s="45"/>
       <c r="X29" s="45"/>
       <c r="Y29" s="45"/>
-      <c r="Z29" s="88"/>
-      <c r="AA29" s="88"/>
-      <c r="AB29" s="88"/>
+      <c r="Z29" s="68"/>
+      <c r="AA29" s="68"/>
+      <c r="AB29" s="68"/>
       <c r="AC29" s="45"/>
       <c r="AD29" s="45"/>
       <c r="AE29" s="45"/>
-      <c r="AF29" s="88"/>
-      <c r="AG29" s="88"/>
-      <c r="AH29" s="88"/>
+      <c r="AF29" s="68"/>
+      <c r="AG29" s="68"/>
+      <c r="AH29" s="68"/>
       <c r="AI29" s="45"/>
       <c r="AJ29" s="45"/>
       <c r="AK29" s="45"/>
@@ -40640,33 +40640,33 @@
       <c r="K30" s="45"/>
       <c r="L30" s="45"/>
       <c r="M30" s="45"/>
-      <c r="N30" s="88" t="s">
+      <c r="N30" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="O30" s="88" t="s">
+      <c r="O30" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P30" s="88" t="s">
+      <c r="P30" s="68" t="s">
         <v>159</v>
       </c>
       <c r="Q30" s="45"/>
       <c r="R30" s="45"/>
       <c r="S30" s="45"/>
-      <c r="T30" s="88"/>
-      <c r="U30" s="88"/>
-      <c r="V30" s="88"/>
+      <c r="T30" s="68"/>
+      <c r="U30" s="68"/>
+      <c r="V30" s="68"/>
       <c r="W30" s="45"/>
       <c r="X30" s="45"/>
       <c r="Y30" s="45"/>
-      <c r="Z30" s="88"/>
-      <c r="AA30" s="88"/>
-      <c r="AB30" s="88"/>
+      <c r="Z30" s="68"/>
+      <c r="AA30" s="68"/>
+      <c r="AB30" s="68"/>
       <c r="AC30" s="45"/>
       <c r="AD30" s="45"/>
       <c r="AE30" s="45"/>
-      <c r="AF30" s="88"/>
-      <c r="AG30" s="88"/>
-      <c r="AH30" s="88"/>
+      <c r="AF30" s="68"/>
+      <c r="AG30" s="68"/>
+      <c r="AH30" s="68"/>
       <c r="AI30" s="45"/>
       <c r="AJ30" s="45"/>
       <c r="AK30" s="45"/>
@@ -40705,33 +40705,33 @@
       <c r="K31" s="45"/>
       <c r="L31" s="45"/>
       <c r="M31" s="45"/>
-      <c r="N31" s="88" t="s">
+      <c r="N31" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="O31" s="88" t="s">
+      <c r="O31" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P31" s="88" t="s">
+      <c r="P31" s="68" t="s">
         <v>156</v>
       </c>
       <c r="Q31" s="45"/>
       <c r="R31" s="45"/>
       <c r="S31" s="45"/>
-      <c r="T31" s="88"/>
-      <c r="U31" s="88"/>
-      <c r="V31" s="88"/>
+      <c r="T31" s="68"/>
+      <c r="U31" s="68"/>
+      <c r="V31" s="68"/>
       <c r="W31" s="45"/>
       <c r="X31" s="45"/>
       <c r="Y31" s="45"/>
-      <c r="Z31" s="88"/>
-      <c r="AA31" s="88"/>
-      <c r="AB31" s="88"/>
+      <c r="Z31" s="68"/>
+      <c r="AA31" s="68"/>
+      <c r="AB31" s="68"/>
       <c r="AC31" s="45"/>
       <c r="AD31" s="45"/>
       <c r="AE31" s="45"/>
-      <c r="AF31" s="88"/>
-      <c r="AG31" s="88"/>
-      <c r="AH31" s="88"/>
+      <c r="AF31" s="68"/>
+      <c r="AG31" s="68"/>
+      <c r="AH31" s="68"/>
       <c r="AI31" s="45"/>
       <c r="AJ31" s="45"/>
       <c r="AK31" s="45"/>
@@ -40770,33 +40770,33 @@
       <c r="K32" s="45"/>
       <c r="L32" s="45"/>
       <c r="M32" s="45"/>
-      <c r="N32" s="88" t="s">
+      <c r="N32" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="O32" s="88" t="s">
+      <c r="O32" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="P32" s="88" t="s">
+      <c r="P32" s="68" t="s">
         <v>108</v>
       </c>
       <c r="Q32" s="45"/>
       <c r="R32" s="45"/>
       <c r="S32" s="45"/>
-      <c r="T32" s="88"/>
-      <c r="U32" s="88"/>
-      <c r="V32" s="88"/>
+      <c r="T32" s="68"/>
+      <c r="U32" s="68"/>
+      <c r="V32" s="68"/>
       <c r="W32" s="45"/>
       <c r="X32" s="45"/>
       <c r="Y32" s="45"/>
-      <c r="Z32" s="88"/>
-      <c r="AA32" s="88"/>
-      <c r="AB32" s="88"/>
+      <c r="Z32" s="68"/>
+      <c r="AA32" s="68"/>
+      <c r="AB32" s="68"/>
       <c r="AC32" s="45"/>
       <c r="AD32" s="45"/>
       <c r="AE32" s="45"/>
-      <c r="AF32" s="88"/>
-      <c r="AG32" s="88"/>
-      <c r="AH32" s="88"/>
+      <c r="AF32" s="68"/>
+      <c r="AG32" s="68"/>
+      <c r="AH32" s="68"/>
       <c r="AI32" s="45"/>
       <c r="AJ32" s="45"/>
       <c r="AK32" s="45"/>
@@ -40835,29 +40835,29 @@
       <c r="K33" s="45"/>
       <c r="L33" s="45"/>
       <c r="M33" s="45"/>
-      <c r="N33" s="88" t="s">
+      <c r="N33" s="68" t="s">
         <v>160</v>
       </c>
-      <c r="O33" s="88"/>
-      <c r="P33" s="88"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
       <c r="Q33" s="45"/>
       <c r="R33" s="45"/>
       <c r="S33" s="45"/>
-      <c r="T33" s="88"/>
-      <c r="U33" s="88"/>
-      <c r="V33" s="88"/>
+      <c r="T33" s="68"/>
+      <c r="U33" s="68"/>
+      <c r="V33" s="68"/>
       <c r="W33" s="45"/>
       <c r="X33" s="45"/>
       <c r="Y33" s="45"/>
-      <c r="Z33" s="88"/>
-      <c r="AA33" s="88"/>
-      <c r="AB33" s="88"/>
+      <c r="Z33" s="68"/>
+      <c r="AA33" s="68"/>
+      <c r="AB33" s="68"/>
       <c r="AC33" s="45"/>
       <c r="AD33" s="45"/>
       <c r="AE33" s="45"/>
-      <c r="AF33" s="88"/>
-      <c r="AG33" s="88"/>
-      <c r="AH33" s="88"/>
+      <c r="AF33" s="68"/>
+      <c r="AG33" s="68"/>
+      <c r="AH33" s="68"/>
       <c r="AI33" s="45"/>
       <c r="AJ33" s="45"/>
       <c r="AK33" s="45"/>
@@ -40896,33 +40896,33 @@
       <c r="K34" s="45"/>
       <c r="L34" s="45"/>
       <c r="M34" s="45"/>
-      <c r="N34" s="88" t="s">
+      <c r="N34" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="O34" s="88" t="s">
+      <c r="O34" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="P34" s="88" t="s">
+      <c r="P34" s="68" t="s">
         <v>128</v>
       </c>
       <c r="Q34" s="45"/>
       <c r="R34" s="45"/>
       <c r="S34" s="45"/>
-      <c r="T34" s="88"/>
-      <c r="U34" s="88"/>
-      <c r="V34" s="88"/>
+      <c r="T34" s="68"/>
+      <c r="U34" s="68"/>
+      <c r="V34" s="68"/>
       <c r="W34" s="45"/>
       <c r="X34" s="45"/>
       <c r="Y34" s="45"/>
-      <c r="Z34" s="88"/>
-      <c r="AA34" s="88"/>
-      <c r="AB34" s="88"/>
+      <c r="Z34" s="68"/>
+      <c r="AA34" s="68"/>
+      <c r="AB34" s="68"/>
       <c r="AC34" s="45"/>
       <c r="AD34" s="45"/>
       <c r="AE34" s="45"/>
-      <c r="AF34" s="88"/>
-      <c r="AG34" s="88"/>
-      <c r="AH34" s="88"/>
+      <c r="AF34" s="68"/>
+      <c r="AG34" s="68"/>
+      <c r="AH34" s="68"/>
       <c r="AI34" s="45"/>
       <c r="AJ34" s="45"/>
       <c r="AK34" s="45"/>
@@ -40961,33 +40961,33 @@
       <c r="K35" s="45"/>
       <c r="L35" s="45"/>
       <c r="M35" s="45"/>
-      <c r="N35" s="88" t="s">
+      <c r="N35" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="O35" s="88" t="s">
+      <c r="O35" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="P35" s="88" t="s">
+      <c r="P35" s="68" t="s">
         <v>128</v>
       </c>
       <c r="Q35" s="45"/>
       <c r="R35" s="45"/>
       <c r="S35" s="45"/>
-      <c r="T35" s="88"/>
-      <c r="U35" s="88"/>
-      <c r="V35" s="88"/>
+      <c r="T35" s="68"/>
+      <c r="U35" s="68"/>
+      <c r="V35" s="68"/>
       <c r="W35" s="45"/>
       <c r="X35" s="45"/>
       <c r="Y35" s="45"/>
-      <c r="Z35" s="88"/>
-      <c r="AA35" s="88"/>
-      <c r="AB35" s="88"/>
+      <c r="Z35" s="68"/>
+      <c r="AA35" s="68"/>
+      <c r="AB35" s="68"/>
       <c r="AC35" s="45"/>
       <c r="AD35" s="45"/>
       <c r="AE35" s="45"/>
-      <c r="AF35" s="88"/>
-      <c r="AG35" s="88"/>
-      <c r="AH35" s="88"/>
+      <c r="AF35" s="68"/>
+      <c r="AG35" s="68"/>
+      <c r="AH35" s="68"/>
       <c r="AI35" s="45"/>
       <c r="AJ35" s="45"/>
       <c r="AK35" s="45"/>
@@ -41026,33 +41026,33 @@
       <c r="K36" s="45"/>
       <c r="L36" s="45"/>
       <c r="M36" s="45"/>
-      <c r="N36" s="88" t="s">
+      <c r="N36" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="O36" s="88" t="s">
+      <c r="O36" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="P36" s="88" t="s">
+      <c r="P36" s="68" t="s">
         <v>128</v>
       </c>
       <c r="Q36" s="45"/>
       <c r="R36" s="45"/>
       <c r="S36" s="45"/>
-      <c r="T36" s="88"/>
-      <c r="U36" s="88"/>
-      <c r="V36" s="88"/>
+      <c r="T36" s="68"/>
+      <c r="U36" s="68"/>
+      <c r="V36" s="68"/>
       <c r="W36" s="45"/>
       <c r="X36" s="45"/>
       <c r="Y36" s="45"/>
-      <c r="Z36" s="88"/>
-      <c r="AA36" s="88"/>
-      <c r="AB36" s="88"/>
+      <c r="Z36" s="68"/>
+      <c r="AA36" s="68"/>
+      <c r="AB36" s="68"/>
       <c r="AC36" s="45"/>
       <c r="AD36" s="45"/>
       <c r="AE36" s="45"/>
-      <c r="AF36" s="88"/>
-      <c r="AG36" s="88"/>
-      <c r="AH36" s="88"/>
+      <c r="AF36" s="68"/>
+      <c r="AG36" s="68"/>
+      <c r="AH36" s="68"/>
       <c r="AI36" s="45"/>
       <c r="AJ36" s="45"/>
       <c r="AK36" s="45"/>
@@ -41091,29 +41091,29 @@
       <c r="K37" s="45"/>
       <c r="L37" s="45"/>
       <c r="M37" s="45"/>
-      <c r="N37" s="88" t="s">
+      <c r="N37" s="68" t="s">
         <v>244</v>
       </c>
-      <c r="O37" s="88"/>
-      <c r="P37" s="88"/>
+      <c r="O37" s="68"/>
+      <c r="P37" s="68"/>
       <c r="Q37" s="45"/>
       <c r="R37" s="45"/>
       <c r="S37" s="45"/>
-      <c r="T37" s="88"/>
-      <c r="U37" s="88"/>
-      <c r="V37" s="88"/>
+      <c r="T37" s="68"/>
+      <c r="U37" s="68"/>
+      <c r="V37" s="68"/>
       <c r="W37" s="45"/>
       <c r="X37" s="45"/>
       <c r="Y37" s="45"/>
-      <c r="Z37" s="88"/>
-      <c r="AA37" s="88"/>
-      <c r="AB37" s="88"/>
+      <c r="Z37" s="68"/>
+      <c r="AA37" s="68"/>
+      <c r="AB37" s="68"/>
       <c r="AC37" s="45"/>
       <c r="AD37" s="45"/>
       <c r="AE37" s="45"/>
-      <c r="AF37" s="88"/>
-      <c r="AG37" s="88"/>
-      <c r="AH37" s="88"/>
+      <c r="AF37" s="68"/>
+      <c r="AG37" s="68"/>
+      <c r="AH37" s="68"/>
       <c r="AI37" s="45"/>
       <c r="AJ37" s="45"/>
       <c r="AK37" s="45"/>
@@ -41154,33 +41154,33 @@
       <c r="K38" s="45"/>
       <c r="L38" s="45"/>
       <c r="M38" s="45"/>
-      <c r="N38" s="88" t="s">
+      <c r="N38" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="O38" s="88" t="s">
+      <c r="O38" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="P38" s="88" t="s">
+      <c r="P38" s="68" t="s">
         <v>134</v>
       </c>
       <c r="Q38" s="45"/>
       <c r="R38" s="45"/>
       <c r="S38" s="45"/>
-      <c r="T38" s="88"/>
-      <c r="U38" s="88"/>
-      <c r="V38" s="88"/>
+      <c r="T38" s="68"/>
+      <c r="U38" s="68"/>
+      <c r="V38" s="68"/>
       <c r="W38" s="45"/>
       <c r="X38" s="45"/>
       <c r="Y38" s="45"/>
-      <c r="Z38" s="88"/>
-      <c r="AA38" s="88"/>
-      <c r="AB38" s="88"/>
+      <c r="Z38" s="68"/>
+      <c r="AA38" s="68"/>
+      <c r="AB38" s="68"/>
       <c r="AC38" s="45"/>
       <c r="AD38" s="45"/>
       <c r="AE38" s="45"/>
-      <c r="AF38" s="88"/>
-      <c r="AG38" s="88"/>
-      <c r="AH38" s="88"/>
+      <c r="AF38" s="68"/>
+      <c r="AG38" s="68"/>
+      <c r="AH38" s="68"/>
       <c r="AI38" s="45"/>
       <c r="AJ38" s="45"/>
       <c r="AK38" s="45"/>
@@ -41219,33 +41219,33 @@
       <c r="K39" s="45"/>
       <c r="L39" s="45"/>
       <c r="M39" s="45"/>
-      <c r="N39" s="88" t="s">
+      <c r="N39" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="O39" s="88" t="s">
+      <c r="O39" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="P39" s="88" t="s">
+      <c r="P39" s="68" t="s">
         <v>275</v>
       </c>
       <c r="Q39" s="45"/>
       <c r="R39" s="45"/>
       <c r="S39" s="45"/>
-      <c r="T39" s="88"/>
-      <c r="U39" s="88"/>
-      <c r="V39" s="88"/>
+      <c r="T39" s="68"/>
+      <c r="U39" s="68"/>
+      <c r="V39" s="68"/>
       <c r="W39" s="45"/>
       <c r="X39" s="45"/>
       <c r="Y39" s="45"/>
-      <c r="Z39" s="88"/>
-      <c r="AA39" s="88"/>
-      <c r="AB39" s="88"/>
+      <c r="Z39" s="68"/>
+      <c r="AA39" s="68"/>
+      <c r="AB39" s="68"/>
       <c r="AC39" s="45"/>
       <c r="AD39" s="45"/>
       <c r="AE39" s="45"/>
-      <c r="AF39" s="88"/>
-      <c r="AG39" s="88"/>
-      <c r="AH39" s="88"/>
+      <c r="AF39" s="68"/>
+      <c r="AG39" s="68"/>
+      <c r="AH39" s="68"/>
       <c r="AI39" s="45"/>
       <c r="AJ39" s="45"/>
       <c r="AK39" s="45"/>
@@ -41284,33 +41284,33 @@
       <c r="K40" s="45"/>
       <c r="L40" s="45"/>
       <c r="M40" s="45"/>
-      <c r="N40" s="88" t="s">
+      <c r="N40" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="O40" s="88" t="s">
+      <c r="O40" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="P40" s="88" t="s">
+      <c r="P40" s="68" t="s">
         <v>275</v>
       </c>
       <c r="Q40" s="45"/>
       <c r="R40" s="45"/>
       <c r="S40" s="45"/>
-      <c r="T40" s="88"/>
-      <c r="U40" s="88"/>
-      <c r="V40" s="88"/>
+      <c r="T40" s="68"/>
+      <c r="U40" s="68"/>
+      <c r="V40" s="68"/>
       <c r="W40" s="45"/>
       <c r="X40" s="45"/>
       <c r="Y40" s="45"/>
-      <c r="Z40" s="88"/>
-      <c r="AA40" s="88"/>
-      <c r="AB40" s="88"/>
+      <c r="Z40" s="68"/>
+      <c r="AA40" s="68"/>
+      <c r="AB40" s="68"/>
       <c r="AC40" s="45"/>
       <c r="AD40" s="45"/>
       <c r="AE40" s="45"/>
-      <c r="AF40" s="88"/>
-      <c r="AG40" s="88"/>
-      <c r="AH40" s="88"/>
+      <c r="AF40" s="68"/>
+      <c r="AG40" s="68"/>
+      <c r="AH40" s="68"/>
       <c r="AI40" s="45"/>
       <c r="AJ40" s="45"/>
       <c r="AK40" s="45"/>
@@ -41345,31 +41345,31 @@
       <c r="K41" s="45"/>
       <c r="L41" s="45"/>
       <c r="M41" s="45"/>
-      <c r="N41" s="88" t="s">
+      <c r="N41" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="O41" s="88"/>
-      <c r="P41" s="88" t="s">
+      <c r="O41" s="68"/>
+      <c r="P41" s="68" t="s">
         <v>276</v>
       </c>
       <c r="Q41" s="45"/>
       <c r="R41" s="45"/>
       <c r="S41" s="45"/>
-      <c r="T41" s="88"/>
-      <c r="U41" s="88"/>
-      <c r="V41" s="88"/>
+      <c r="T41" s="68"/>
+      <c r="U41" s="68"/>
+      <c r="V41" s="68"/>
       <c r="W41" s="45"/>
       <c r="X41" s="45"/>
       <c r="Y41" s="45"/>
-      <c r="Z41" s="88"/>
-      <c r="AA41" s="88"/>
-      <c r="AB41" s="88"/>
+      <c r="Z41" s="68"/>
+      <c r="AA41" s="68"/>
+      <c r="AB41" s="68"/>
       <c r="AC41" s="45"/>
       <c r="AD41" s="45"/>
       <c r="AE41" s="45"/>
-      <c r="AF41" s="88"/>
-      <c r="AG41" s="88"/>
-      <c r="AH41" s="88"/>
+      <c r="AF41" s="68"/>
+      <c r="AG41" s="68"/>
+      <c r="AH41" s="68"/>
       <c r="AI41" s="45"/>
       <c r="AJ41" s="45"/>
       <c r="AK41" s="45"/>
@@ -41408,33 +41408,33 @@
       <c r="K42" s="45"/>
       <c r="L42" s="45"/>
       <c r="M42" s="45"/>
-      <c r="N42" s="88" t="s">
+      <c r="N42" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="O42" s="88" t="s">
+      <c r="O42" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="P42" s="88" t="s">
+      <c r="P42" s="68" t="s">
         <v>116</v>
       </c>
       <c r="Q42" s="45"/>
       <c r="R42" s="45"/>
       <c r="S42" s="45"/>
-      <c r="T42" s="88"/>
-      <c r="U42" s="88"/>
-      <c r="V42" s="88"/>
+      <c r="T42" s="68"/>
+      <c r="U42" s="68"/>
+      <c r="V42" s="68"/>
       <c r="W42" s="45"/>
       <c r="X42" s="45"/>
       <c r="Y42" s="45"/>
-      <c r="Z42" s="88"/>
-      <c r="AA42" s="88"/>
-      <c r="AB42" s="88"/>
+      <c r="Z42" s="68"/>
+      <c r="AA42" s="68"/>
+      <c r="AB42" s="68"/>
       <c r="AC42" s="45"/>
       <c r="AD42" s="45"/>
       <c r="AE42" s="45"/>
-      <c r="AF42" s="88"/>
-      <c r="AG42" s="88"/>
-      <c r="AH42" s="88"/>
+      <c r="AF42" s="68"/>
+      <c r="AG42" s="68"/>
+      <c r="AH42" s="68"/>
       <c r="AI42" s="45"/>
       <c r="AJ42" s="45"/>
       <c r="AK42" s="45"/>
@@ -41473,33 +41473,33 @@
       <c r="K43" s="45"/>
       <c r="L43" s="45"/>
       <c r="M43" s="45"/>
-      <c r="N43" s="88" t="s">
+      <c r="N43" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="O43" s="88" t="s">
+      <c r="O43" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="P43" s="88" t="s">
+      <c r="P43" s="68" t="s">
         <v>275</v>
       </c>
       <c r="Q43" s="45"/>
       <c r="R43" s="45"/>
       <c r="S43" s="45"/>
-      <c r="T43" s="88"/>
-      <c r="U43" s="88"/>
-      <c r="V43" s="88"/>
+      <c r="T43" s="68"/>
+      <c r="U43" s="68"/>
+      <c r="V43" s="68"/>
       <c r="W43" s="45"/>
       <c r="X43" s="45"/>
       <c r="Y43" s="45"/>
-      <c r="Z43" s="88"/>
-      <c r="AA43" s="88"/>
-      <c r="AB43" s="88"/>
+      <c r="Z43" s="68"/>
+      <c r="AA43" s="68"/>
+      <c r="AB43" s="68"/>
       <c r="AC43" s="45"/>
       <c r="AD43" s="45"/>
       <c r="AE43" s="45"/>
-      <c r="AF43" s="88"/>
-      <c r="AG43" s="88"/>
-      <c r="AH43" s="88"/>
+      <c r="AF43" s="68"/>
+      <c r="AG43" s="68"/>
+      <c r="AH43" s="68"/>
       <c r="AI43" s="45"/>
       <c r="AJ43" s="45"/>
       <c r="AK43" s="45"/>
@@ -41538,29 +41538,29 @@
       <c r="K44" s="45"/>
       <c r="L44" s="45"/>
       <c r="M44" s="45"/>
-      <c r="N44" s="88"/>
-      <c r="O44" s="88"/>
-      <c r="P44" s="88"/>
+      <c r="N44" s="68"/>
+      <c r="O44" s="68"/>
+      <c r="P44" s="68"/>
       <c r="Q44" s="45" t="s">
         <v>269</v>
       </c>
       <c r="R44" s="45"/>
       <c r="S44" s="45"/>
-      <c r="T44" s="88"/>
-      <c r="U44" s="88"/>
-      <c r="V44" s="88"/>
+      <c r="T44" s="68"/>
+      <c r="U44" s="68"/>
+      <c r="V44" s="68"/>
       <c r="W44" s="45"/>
       <c r="X44" s="45"/>
       <c r="Y44" s="45"/>
-      <c r="Z44" s="88"/>
-      <c r="AA44" s="88"/>
-      <c r="AB44" s="88"/>
+      <c r="Z44" s="68"/>
+      <c r="AA44" s="68"/>
+      <c r="AB44" s="68"/>
       <c r="AC44" s="45"/>
       <c r="AD44" s="45"/>
       <c r="AE44" s="45"/>
-      <c r="AF44" s="88"/>
-      <c r="AG44" s="88"/>
-      <c r="AH44" s="88"/>
+      <c r="AF44" s="68"/>
+      <c r="AG44" s="68"/>
+      <c r="AH44" s="68"/>
       <c r="AI44" s="45"/>
       <c r="AJ44" s="45"/>
       <c r="AK44" s="45"/>
@@ -41601,29 +41601,29 @@
       <c r="K45" s="45"/>
       <c r="L45" s="45"/>
       <c r="M45" s="45"/>
-      <c r="N45" s="88"/>
-      <c r="O45" s="88"/>
-      <c r="P45" s="88"/>
+      <c r="N45" s="68"/>
+      <c r="O45" s="68"/>
+      <c r="P45" s="68"/>
       <c r="Q45" s="45" t="s">
         <v>269</v>
       </c>
       <c r="R45" s="45"/>
       <c r="S45" s="45"/>
-      <c r="T45" s="88"/>
-      <c r="U45" s="88"/>
-      <c r="V45" s="88"/>
+      <c r="T45" s="68"/>
+      <c r="U45" s="68"/>
+      <c r="V45" s="68"/>
       <c r="W45" s="45"/>
       <c r="X45" s="45"/>
       <c r="Y45" s="45"/>
-      <c r="Z45" s="88"/>
-      <c r="AA45" s="88"/>
-      <c r="AB45" s="88"/>
+      <c r="Z45" s="68"/>
+      <c r="AA45" s="68"/>
+      <c r="AB45" s="68"/>
       <c r="AC45" s="45"/>
       <c r="AD45" s="45"/>
       <c r="AE45" s="45"/>
-      <c r="AF45" s="88"/>
-      <c r="AG45" s="88"/>
-      <c r="AH45" s="88"/>
+      <c r="AF45" s="68"/>
+      <c r="AG45" s="68"/>
+      <c r="AH45" s="68"/>
       <c r="AI45" s="45"/>
       <c r="AJ45" s="45"/>
       <c r="AK45" s="45"/>
@@ -41662,29 +41662,29 @@
       <c r="K46" s="45"/>
       <c r="L46" s="45"/>
       <c r="M46" s="45"/>
-      <c r="N46" s="88"/>
-      <c r="O46" s="88"/>
-      <c r="P46" s="88"/>
+      <c r="N46" s="68"/>
+      <c r="O46" s="68"/>
+      <c r="P46" s="68"/>
       <c r="Q46" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R46" s="45"/>
       <c r="S46" s="45"/>
-      <c r="T46" s="88"/>
-      <c r="U46" s="88"/>
-      <c r="V46" s="88"/>
+      <c r="T46" s="68"/>
+      <c r="U46" s="68"/>
+      <c r="V46" s="68"/>
       <c r="W46" s="45"/>
       <c r="X46" s="45"/>
       <c r="Y46" s="45"/>
-      <c r="Z46" s="88"/>
-      <c r="AA46" s="88"/>
-      <c r="AB46" s="88"/>
+      <c r="Z46" s="68"/>
+      <c r="AA46" s="68"/>
+      <c r="AB46" s="68"/>
       <c r="AC46" s="45"/>
       <c r="AD46" s="45"/>
       <c r="AE46" s="45"/>
-      <c r="AF46" s="88"/>
-      <c r="AG46" s="88"/>
-      <c r="AH46" s="88"/>
+      <c r="AF46" s="68"/>
+      <c r="AG46" s="68"/>
+      <c r="AH46" s="68"/>
       <c r="AI46" s="45"/>
       <c r="AJ46" s="45"/>
       <c r="AK46" s="45"/>
@@ -41723,29 +41723,29 @@
       <c r="K47" s="45"/>
       <c r="L47" s="45"/>
       <c r="M47" s="45"/>
-      <c r="N47" s="88"/>
-      <c r="O47" s="88"/>
-      <c r="P47" s="88"/>
+      <c r="N47" s="68"/>
+      <c r="O47" s="68"/>
+      <c r="P47" s="68"/>
       <c r="Q47" s="45" t="s">
         <v>159</v>
       </c>
       <c r="R47" s="45"/>
       <c r="S47" s="45"/>
-      <c r="T47" s="88"/>
-      <c r="U47" s="88"/>
-      <c r="V47" s="88"/>
+      <c r="T47" s="68"/>
+      <c r="U47" s="68"/>
+      <c r="V47" s="68"/>
       <c r="W47" s="45"/>
       <c r="X47" s="45"/>
       <c r="Y47" s="45"/>
-      <c r="Z47" s="88"/>
-      <c r="AA47" s="88"/>
-      <c r="AB47" s="88"/>
+      <c r="Z47" s="68"/>
+      <c r="AA47" s="68"/>
+      <c r="AB47" s="68"/>
       <c r="AC47" s="45"/>
       <c r="AD47" s="45"/>
       <c r="AE47" s="45"/>
-      <c r="AF47" s="88"/>
-      <c r="AG47" s="88"/>
-      <c r="AH47" s="88"/>
+      <c r="AF47" s="68"/>
+      <c r="AG47" s="68"/>
+      <c r="AH47" s="68"/>
       <c r="AI47" s="45"/>
       <c r="AJ47" s="45"/>
       <c r="AK47" s="45"/>
@@ -41784,29 +41784,29 @@
       <c r="K48" s="45"/>
       <c r="L48" s="45"/>
       <c r="M48" s="45"/>
-      <c r="N48" s="88"/>
-      <c r="O48" s="88"/>
-      <c r="P48" s="88"/>
+      <c r="N48" s="68"/>
+      <c r="O48" s="68"/>
+      <c r="P48" s="68"/>
       <c r="Q48" s="45" t="s">
         <v>159</v>
       </c>
       <c r="R48" s="45"/>
       <c r="S48" s="45"/>
-      <c r="T48" s="88"/>
-      <c r="U48" s="88"/>
-      <c r="V48" s="88"/>
+      <c r="T48" s="68"/>
+      <c r="U48" s="68"/>
+      <c r="V48" s="68"/>
       <c r="W48" s="45"/>
       <c r="X48" s="45"/>
       <c r="Y48" s="45"/>
-      <c r="Z48" s="88"/>
-      <c r="AA48" s="88"/>
-      <c r="AB48" s="88"/>
+      <c r="Z48" s="68"/>
+      <c r="AA48" s="68"/>
+      <c r="AB48" s="68"/>
       <c r="AC48" s="45"/>
       <c r="AD48" s="45"/>
       <c r="AE48" s="45"/>
-      <c r="AF48" s="88"/>
-      <c r="AG48" s="88"/>
-      <c r="AH48" s="88"/>
+      <c r="AF48" s="68"/>
+      <c r="AG48" s="68"/>
+      <c r="AH48" s="68"/>
       <c r="AI48" s="45"/>
       <c r="AJ48" s="45"/>
       <c r="AK48" s="45"/>
@@ -41845,29 +41845,29 @@
       <c r="K49" s="45"/>
       <c r="L49" s="45"/>
       <c r="M49" s="45"/>
-      <c r="N49" s="88"/>
-      <c r="O49" s="88"/>
-      <c r="P49" s="88"/>
+      <c r="N49" s="68"/>
+      <c r="O49" s="68"/>
+      <c r="P49" s="68"/>
       <c r="Q49" s="45" t="s">
         <v>159</v>
       </c>
       <c r="R49" s="45"/>
       <c r="S49" s="45"/>
-      <c r="T49" s="88"/>
-      <c r="U49" s="88"/>
-      <c r="V49" s="88"/>
+      <c r="T49" s="68"/>
+      <c r="U49" s="68"/>
+      <c r="V49" s="68"/>
       <c r="W49" s="45"/>
       <c r="X49" s="45"/>
       <c r="Y49" s="45"/>
-      <c r="Z49" s="88"/>
-      <c r="AA49" s="88"/>
-      <c r="AB49" s="88"/>
+      <c r="Z49" s="68"/>
+      <c r="AA49" s="68"/>
+      <c r="AB49" s="68"/>
       <c r="AC49" s="45"/>
       <c r="AD49" s="45"/>
       <c r="AE49" s="45"/>
-      <c r="AF49" s="88"/>
-      <c r="AG49" s="88"/>
-      <c r="AH49" s="88"/>
+      <c r="AF49" s="68"/>
+      <c r="AG49" s="68"/>
+      <c r="AH49" s="68"/>
       <c r="AI49" s="45"/>
       <c r="AJ49" s="45"/>
       <c r="AK49" s="45"/>
@@ -41908,29 +41908,29 @@
       <c r="K50" s="45"/>
       <c r="L50" s="45"/>
       <c r="M50" s="45"/>
-      <c r="N50" s="88"/>
-      <c r="O50" s="88"/>
-      <c r="P50" s="88"/>
+      <c r="N50" s="68"/>
+      <c r="O50" s="68"/>
+      <c r="P50" s="68"/>
       <c r="Q50" s="45" t="s">
         <v>159</v>
       </c>
       <c r="R50" s="45"/>
       <c r="S50" s="45"/>
-      <c r="T50" s="88"/>
-      <c r="U50" s="88"/>
-      <c r="V50" s="88"/>
+      <c r="T50" s="68"/>
+      <c r="U50" s="68"/>
+      <c r="V50" s="68"/>
       <c r="W50" s="45"/>
       <c r="X50" s="45"/>
       <c r="Y50" s="45"/>
-      <c r="Z50" s="88"/>
-      <c r="AA50" s="88"/>
-      <c r="AB50" s="88"/>
+      <c r="Z50" s="68"/>
+      <c r="AA50" s="68"/>
+      <c r="AB50" s="68"/>
       <c r="AC50" s="45"/>
       <c r="AD50" s="45"/>
       <c r="AE50" s="45"/>
-      <c r="AF50" s="88"/>
-      <c r="AG50" s="88"/>
-      <c r="AH50" s="88"/>
+      <c r="AF50" s="68"/>
+      <c r="AG50" s="68"/>
+      <c r="AH50" s="68"/>
       <c r="AI50" s="45"/>
       <c r="AJ50" s="45"/>
       <c r="AK50" s="45"/>
@@ -41969,29 +41969,29 @@
       <c r="K51" s="45"/>
       <c r="L51" s="45"/>
       <c r="M51" s="45"/>
-      <c r="N51" s="88"/>
-      <c r="O51" s="88"/>
-      <c r="P51" s="88"/>
+      <c r="N51" s="68"/>
+      <c r="O51" s="68"/>
+      <c r="P51" s="68"/>
       <c r="Q51" s="45" t="s">
         <v>156</v>
       </c>
       <c r="R51" s="45"/>
       <c r="S51" s="45"/>
-      <c r="T51" s="88"/>
-      <c r="U51" s="88"/>
-      <c r="V51" s="88"/>
+      <c r="T51" s="68"/>
+      <c r="U51" s="68"/>
+      <c r="V51" s="68"/>
       <c r="W51" s="45"/>
       <c r="X51" s="45"/>
       <c r="Y51" s="45"/>
-      <c r="Z51" s="88"/>
-      <c r="AA51" s="88"/>
-      <c r="AB51" s="88"/>
+      <c r="Z51" s="68"/>
+      <c r="AA51" s="68"/>
+      <c r="AB51" s="68"/>
       <c r="AC51" s="45"/>
       <c r="AD51" s="45"/>
       <c r="AE51" s="45"/>
-      <c r="AF51" s="88"/>
-      <c r="AG51" s="88"/>
-      <c r="AH51" s="88"/>
+      <c r="AF51" s="68"/>
+      <c r="AG51" s="68"/>
+      <c r="AH51" s="68"/>
       <c r="AI51" s="45"/>
       <c r="AJ51" s="45"/>
       <c r="AK51" s="45"/>
@@ -42030,29 +42030,29 @@
       <c r="K52" s="45"/>
       <c r="L52" s="45"/>
       <c r="M52" s="45"/>
-      <c r="N52" s="88"/>
-      <c r="O52" s="88"/>
-      <c r="P52" s="88"/>
+      <c r="N52" s="68"/>
+      <c r="O52" s="68"/>
+      <c r="P52" s="68"/>
       <c r="Q52" s="45" t="s">
         <v>156</v>
       </c>
       <c r="R52" s="45"/>
       <c r="S52" s="45"/>
-      <c r="T52" s="88"/>
-      <c r="U52" s="88"/>
-      <c r="V52" s="88"/>
+      <c r="T52" s="68"/>
+      <c r="U52" s="68"/>
+      <c r="V52" s="68"/>
       <c r="W52" s="45"/>
       <c r="X52" s="45"/>
       <c r="Y52" s="45"/>
-      <c r="Z52" s="88"/>
-      <c r="AA52" s="88"/>
-      <c r="AB52" s="88"/>
+      <c r="Z52" s="68"/>
+      <c r="AA52" s="68"/>
+      <c r="AB52" s="68"/>
       <c r="AC52" s="45"/>
       <c r="AD52" s="45"/>
       <c r="AE52" s="45"/>
-      <c r="AF52" s="88"/>
-      <c r="AG52" s="88"/>
-      <c r="AH52" s="88"/>
+      <c r="AF52" s="68"/>
+      <c r="AG52" s="68"/>
+      <c r="AH52" s="68"/>
       <c r="AI52" s="45"/>
       <c r="AJ52" s="45"/>
       <c r="AK52" s="45"/>
@@ -42093,29 +42093,29 @@
       <c r="K53" s="45"/>
       <c r="L53" s="45"/>
       <c r="M53" s="45"/>
-      <c r="N53" s="88"/>
-      <c r="O53" s="88"/>
-      <c r="P53" s="88"/>
+      <c r="N53" s="68"/>
+      <c r="O53" s="68"/>
+      <c r="P53" s="68"/>
       <c r="Q53" s="45" t="s">
         <v>164</v>
       </c>
       <c r="R53" s="45"/>
       <c r="S53" s="45"/>
-      <c r="T53" s="88"/>
-      <c r="U53" s="88"/>
-      <c r="V53" s="88"/>
+      <c r="T53" s="68"/>
+      <c r="U53" s="68"/>
+      <c r="V53" s="68"/>
       <c r="W53" s="45"/>
       <c r="X53" s="45"/>
       <c r="Y53" s="45"/>
-      <c r="Z53" s="88"/>
-      <c r="AA53" s="88"/>
-      <c r="AB53" s="88"/>
+      <c r="Z53" s="68"/>
+      <c r="AA53" s="68"/>
+      <c r="AB53" s="68"/>
       <c r="AC53" s="45"/>
       <c r="AD53" s="45"/>
       <c r="AE53" s="45"/>
-      <c r="AF53" s="88"/>
-      <c r="AG53" s="88"/>
-      <c r="AH53" s="88"/>
+      <c r="AF53" s="68"/>
+      <c r="AG53" s="68"/>
+      <c r="AH53" s="68"/>
       <c r="AI53" s="45"/>
       <c r="AJ53" s="45"/>
       <c r="AK53" s="45"/>
@@ -42149,29 +42149,29 @@
       <c r="K54" s="45"/>
       <c r="L54" s="45"/>
       <c r="M54" s="45"/>
-      <c r="N54" s="88"/>
-      <c r="O54" s="88"/>
-      <c r="P54" s="88"/>
+      <c r="N54" s="68"/>
+      <c r="O54" s="68"/>
+      <c r="P54" s="68"/>
       <c r="Q54" s="45" t="s">
         <v>158</v>
       </c>
       <c r="R54" s="45"/>
       <c r="S54" s="45"/>
-      <c r="T54" s="88"/>
-      <c r="U54" s="88"/>
-      <c r="V54" s="88"/>
+      <c r="T54" s="68"/>
+      <c r="U54" s="68"/>
+      <c r="V54" s="68"/>
       <c r="W54" s="45"/>
       <c r="X54" s="45"/>
       <c r="Y54" s="45"/>
-      <c r="Z54" s="88"/>
-      <c r="AA54" s="88"/>
-      <c r="AB54" s="88"/>
+      <c r="Z54" s="68"/>
+      <c r="AA54" s="68"/>
+      <c r="AB54" s="68"/>
       <c r="AC54" s="45"/>
       <c r="AD54" s="45"/>
       <c r="AE54" s="45"/>
-      <c r="AF54" s="88"/>
-      <c r="AG54" s="88"/>
-      <c r="AH54" s="88"/>
+      <c r="AF54" s="68"/>
+      <c r="AG54" s="68"/>
+      <c r="AH54" s="68"/>
       <c r="AI54" s="45"/>
       <c r="AJ54" s="45"/>
       <c r="AK54" s="45"/>
@@ -42210,29 +42210,29 @@
       <c r="K55" s="45"/>
       <c r="L55" s="45"/>
       <c r="M55" s="45"/>
-      <c r="N55" s="88"/>
-      <c r="O55" s="88"/>
-      <c r="P55" s="88"/>
+      <c r="N55" s="68"/>
+      <c r="O55" s="68"/>
+      <c r="P55" s="68"/>
       <c r="Q55" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R55" s="45"/>
       <c r="S55" s="45"/>
-      <c r="T55" s="88"/>
-      <c r="U55" s="88"/>
-      <c r="V55" s="88"/>
+      <c r="T55" s="68"/>
+      <c r="U55" s="68"/>
+      <c r="V55" s="68"/>
       <c r="W55" s="45"/>
       <c r="X55" s="45"/>
       <c r="Y55" s="45"/>
-      <c r="Z55" s="88"/>
-      <c r="AA55" s="88"/>
-      <c r="AB55" s="88"/>
+      <c r="Z55" s="68"/>
+      <c r="AA55" s="68"/>
+      <c r="AB55" s="68"/>
       <c r="AC55" s="45"/>
       <c r="AD55" s="45"/>
       <c r="AE55" s="45"/>
-      <c r="AF55" s="88"/>
-      <c r="AG55" s="88"/>
-      <c r="AH55" s="88"/>
+      <c r="AF55" s="68"/>
+      <c r="AG55" s="68"/>
+      <c r="AH55" s="68"/>
       <c r="AI55" s="45"/>
       <c r="AJ55" s="45"/>
       <c r="AK55" s="45"/>
@@ -42264,29 +42264,29 @@
       <c r="K56" s="45"/>
       <c r="L56" s="45"/>
       <c r="M56" s="45"/>
-      <c r="N56" s="88"/>
-      <c r="O56" s="88"/>
-      <c r="P56" s="88"/>
+      <c r="N56" s="68"/>
+      <c r="O56" s="68"/>
+      <c r="P56" s="68"/>
       <c r="Q56" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R56" s="45"/>
       <c r="S56" s="45"/>
-      <c r="T56" s="88"/>
-      <c r="U56" s="88"/>
-      <c r="V56" s="88"/>
+      <c r="T56" s="68"/>
+      <c r="U56" s="68"/>
+      <c r="V56" s="68"/>
       <c r="W56" s="45"/>
       <c r="X56" s="45"/>
       <c r="Y56" s="45"/>
-      <c r="Z56" s="88"/>
-      <c r="AA56" s="88"/>
-      <c r="AB56" s="88"/>
+      <c r="Z56" s="68"/>
+      <c r="AA56" s="68"/>
+      <c r="AB56" s="68"/>
       <c r="AC56" s="45"/>
       <c r="AD56" s="45"/>
       <c r="AE56" s="45"/>
-      <c r="AF56" s="88"/>
-      <c r="AG56" s="88"/>
-      <c r="AH56" s="88"/>
+      <c r="AF56" s="68"/>
+      <c r="AG56" s="68"/>
+      <c r="AH56" s="68"/>
       <c r="AI56" s="45"/>
       <c r="AJ56" s="45"/>
       <c r="AK56" s="45"/>
@@ -42318,29 +42318,29 @@
       <c r="K57" s="45"/>
       <c r="L57" s="45"/>
       <c r="M57" s="45"/>
-      <c r="N57" s="88"/>
-      <c r="O57" s="88"/>
-      <c r="P57" s="88"/>
+      <c r="N57" s="68"/>
+      <c r="O57" s="68"/>
+      <c r="P57" s="68"/>
       <c r="Q57" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R57" s="45"/>
       <c r="S57" s="45"/>
-      <c r="T57" s="88"/>
-      <c r="U57" s="88"/>
-      <c r="V57" s="88"/>
+      <c r="T57" s="68"/>
+      <c r="U57" s="68"/>
+      <c r="V57" s="68"/>
       <c r="W57" s="45"/>
       <c r="X57" s="45"/>
       <c r="Y57" s="45"/>
-      <c r="Z57" s="88"/>
-      <c r="AA57" s="88"/>
-      <c r="AB57" s="88"/>
+      <c r="Z57" s="68"/>
+      <c r="AA57" s="68"/>
+      <c r="AB57" s="68"/>
       <c r="AC57" s="45"/>
       <c r="AD57" s="45"/>
       <c r="AE57" s="45"/>
-      <c r="AF57" s="88"/>
-      <c r="AG57" s="88"/>
-      <c r="AH57" s="88"/>
+      <c r="AF57" s="68"/>
+      <c r="AG57" s="68"/>
+      <c r="AH57" s="68"/>
       <c r="AI57" s="45"/>
       <c r="AJ57" s="45"/>
       <c r="AK57" s="45"/>
@@ -42372,29 +42372,29 @@
       <c r="K58" s="45"/>
       <c r="L58" s="45"/>
       <c r="M58" s="45"/>
-      <c r="N58" s="88"/>
-      <c r="O58" s="88"/>
-      <c r="P58" s="88"/>
+      <c r="N58" s="68"/>
+      <c r="O58" s="68"/>
+      <c r="P58" s="68"/>
       <c r="Q58" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R58" s="45"/>
       <c r="S58" s="45"/>
-      <c r="T58" s="88"/>
-      <c r="U58" s="88"/>
-      <c r="V58" s="88"/>
+      <c r="T58" s="68"/>
+      <c r="U58" s="68"/>
+      <c r="V58" s="68"/>
       <c r="W58" s="45"/>
       <c r="X58" s="45"/>
       <c r="Y58" s="45"/>
-      <c r="Z58" s="88"/>
-      <c r="AA58" s="88"/>
-      <c r="AB58" s="88"/>
+      <c r="Z58" s="68"/>
+      <c r="AA58" s="68"/>
+      <c r="AB58" s="68"/>
       <c r="AC58" s="45"/>
       <c r="AD58" s="45"/>
       <c r="AE58" s="45"/>
-      <c r="AF58" s="88"/>
-      <c r="AG58" s="88"/>
-      <c r="AH58" s="88"/>
+      <c r="AF58" s="68"/>
+      <c r="AG58" s="68"/>
+      <c r="AH58" s="68"/>
       <c r="AI58" s="45"/>
       <c r="AJ58" s="45"/>
       <c r="AK58" s="45"/>
@@ -42428,29 +42428,29 @@
       <c r="K59" s="45"/>
       <c r="L59" s="45"/>
       <c r="M59" s="45"/>
-      <c r="N59" s="88"/>
-      <c r="O59" s="88"/>
-      <c r="P59" s="88"/>
+      <c r="N59" s="68"/>
+      <c r="O59" s="68"/>
+      <c r="P59" s="68"/>
       <c r="Q59" s="45" t="s">
         <v>159</v>
       </c>
       <c r="R59" s="45"/>
       <c r="S59" s="45"/>
-      <c r="T59" s="88"/>
-      <c r="U59" s="88"/>
-      <c r="V59" s="88"/>
+      <c r="T59" s="68"/>
+      <c r="U59" s="68"/>
+      <c r="V59" s="68"/>
       <c r="W59" s="45"/>
       <c r="X59" s="45"/>
       <c r="Y59" s="45"/>
-      <c r="Z59" s="88"/>
-      <c r="AA59" s="88"/>
-      <c r="AB59" s="88"/>
+      <c r="Z59" s="68"/>
+      <c r="AA59" s="68"/>
+      <c r="AB59" s="68"/>
       <c r="AC59" s="45"/>
       <c r="AD59" s="45"/>
       <c r="AE59" s="45"/>
-      <c r="AF59" s="88"/>
-      <c r="AG59" s="88"/>
-      <c r="AH59" s="88"/>
+      <c r="AF59" s="68"/>
+      <c r="AG59" s="68"/>
+      <c r="AH59" s="68"/>
       <c r="AI59" s="45"/>
       <c r="AJ59" s="45"/>
       <c r="AK59" s="45"/>
@@ -42482,29 +42482,29 @@
       <c r="K60" s="45"/>
       <c r="L60" s="45"/>
       <c r="M60" s="45"/>
-      <c r="N60" s="88"/>
-      <c r="O60" s="88"/>
-      <c r="P60" s="88"/>
+      <c r="N60" s="68"/>
+      <c r="O60" s="68"/>
+      <c r="P60" s="68"/>
       <c r="Q60" s="45" t="s">
         <v>156</v>
       </c>
       <c r="R60" s="45"/>
       <c r="S60" s="45"/>
-      <c r="T60" s="88"/>
-      <c r="U60" s="88"/>
-      <c r="V60" s="88"/>
+      <c r="T60" s="68"/>
+      <c r="U60" s="68"/>
+      <c r="V60" s="68"/>
       <c r="W60" s="45"/>
       <c r="X60" s="45"/>
       <c r="Y60" s="45"/>
-      <c r="Z60" s="88"/>
-      <c r="AA60" s="88"/>
-      <c r="AB60" s="88"/>
+      <c r="Z60" s="68"/>
+      <c r="AA60" s="68"/>
+      <c r="AB60" s="68"/>
       <c r="AC60" s="45"/>
       <c r="AD60" s="45"/>
       <c r="AE60" s="45"/>
-      <c r="AF60" s="88"/>
-      <c r="AG60" s="88"/>
-      <c r="AH60" s="88"/>
+      <c r="AF60" s="68"/>
+      <c r="AG60" s="68"/>
+      <c r="AH60" s="68"/>
       <c r="AI60" s="45"/>
       <c r="AJ60" s="45"/>
       <c r="AK60" s="45"/>
@@ -42536,29 +42536,29 @@
       <c r="K61" s="45"/>
       <c r="L61" s="45"/>
       <c r="M61" s="45"/>
-      <c r="N61" s="88"/>
-      <c r="O61" s="88"/>
-      <c r="P61" s="88"/>
+      <c r="N61" s="68"/>
+      <c r="O61" s="68"/>
+      <c r="P61" s="68"/>
       <c r="Q61" s="45" t="s">
         <v>156</v>
       </c>
       <c r="R61" s="45"/>
       <c r="S61" s="45"/>
-      <c r="T61" s="88"/>
-      <c r="U61" s="88"/>
-      <c r="V61" s="88"/>
+      <c r="T61" s="68"/>
+      <c r="U61" s="68"/>
+      <c r="V61" s="68"/>
       <c r="W61" s="45"/>
       <c r="X61" s="45"/>
       <c r="Y61" s="45"/>
-      <c r="Z61" s="88"/>
-      <c r="AA61" s="88"/>
-      <c r="AB61" s="88"/>
+      <c r="Z61" s="68"/>
+      <c r="AA61" s="68"/>
+      <c r="AB61" s="68"/>
       <c r="AC61" s="45"/>
       <c r="AD61" s="45"/>
       <c r="AE61" s="45"/>
-      <c r="AF61" s="88"/>
-      <c r="AG61" s="88"/>
-      <c r="AH61" s="88"/>
+      <c r="AF61" s="68"/>
+      <c r="AG61" s="68"/>
+      <c r="AH61" s="68"/>
       <c r="AI61" s="45"/>
       <c r="AJ61" s="45"/>
       <c r="AK61" s="45"/>
@@ -42592,29 +42592,29 @@
       <c r="K62" s="45"/>
       <c r="L62" s="45"/>
       <c r="M62" s="45"/>
-      <c r="N62" s="88"/>
-      <c r="O62" s="88"/>
-      <c r="P62" s="88"/>
+      <c r="N62" s="68"/>
+      <c r="O62" s="68"/>
+      <c r="P62" s="68"/>
       <c r="Q62" s="45" t="s">
         <v>271</v>
       </c>
       <c r="R62" s="45"/>
       <c r="S62" s="45"/>
-      <c r="T62" s="88"/>
-      <c r="U62" s="88"/>
-      <c r="V62" s="88"/>
+      <c r="T62" s="68"/>
+      <c r="U62" s="68"/>
+      <c r="V62" s="68"/>
       <c r="W62" s="45"/>
       <c r="X62" s="45"/>
       <c r="Y62" s="45"/>
-      <c r="Z62" s="88"/>
-      <c r="AA62" s="88"/>
-      <c r="AB62" s="88"/>
+      <c r="Z62" s="68"/>
+      <c r="AA62" s="68"/>
+      <c r="AB62" s="68"/>
       <c r="AC62" s="45"/>
       <c r="AD62" s="45"/>
       <c r="AE62" s="45"/>
-      <c r="AF62" s="88"/>
-      <c r="AG62" s="88"/>
-      <c r="AH62" s="88"/>
+      <c r="AF62" s="68"/>
+      <c r="AG62" s="68"/>
+      <c r="AH62" s="68"/>
       <c r="AI62" s="45"/>
       <c r="AJ62" s="45"/>
       <c r="AK62" s="45"/>
@@ -42655,29 +42655,29 @@
       <c r="K63" s="45"/>
       <c r="L63" s="45"/>
       <c r="M63" s="45"/>
-      <c r="N63" s="88"/>
-      <c r="O63" s="88"/>
-      <c r="P63" s="88"/>
+      <c r="N63" s="68"/>
+      <c r="O63" s="68"/>
+      <c r="P63" s="68"/>
       <c r="Q63" s="45" t="s">
         <v>159</v>
       </c>
       <c r="R63" s="45"/>
       <c r="S63" s="45"/>
-      <c r="T63" s="88"/>
-      <c r="U63" s="88"/>
-      <c r="V63" s="88"/>
+      <c r="T63" s="68"/>
+      <c r="U63" s="68"/>
+      <c r="V63" s="68"/>
       <c r="W63" s="45"/>
       <c r="X63" s="45"/>
       <c r="Y63" s="45"/>
-      <c r="Z63" s="88"/>
-      <c r="AA63" s="88"/>
-      <c r="AB63" s="88"/>
+      <c r="Z63" s="68"/>
+      <c r="AA63" s="68"/>
+      <c r="AB63" s="68"/>
       <c r="AC63" s="45"/>
       <c r="AD63" s="45"/>
       <c r="AE63" s="45"/>
-      <c r="AF63" s="88"/>
-      <c r="AG63" s="88"/>
-      <c r="AH63" s="88"/>
+      <c r="AF63" s="68"/>
+      <c r="AG63" s="68"/>
+      <c r="AH63" s="68"/>
       <c r="AI63" s="45"/>
       <c r="AJ63" s="45"/>
       <c r="AK63" s="45"/>
@@ -42716,29 +42716,29 @@
       <c r="K64" s="45"/>
       <c r="L64" s="45"/>
       <c r="M64" s="45"/>
-      <c r="N64" s="88"/>
-      <c r="O64" s="88"/>
-      <c r="P64" s="88"/>
+      <c r="N64" s="68"/>
+      <c r="O64" s="68"/>
+      <c r="P64" s="68"/>
       <c r="Q64" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R64" s="45"/>
       <c r="S64" s="45"/>
-      <c r="T64" s="88"/>
-      <c r="U64" s="88"/>
-      <c r="V64" s="88"/>
+      <c r="T64" s="68"/>
+      <c r="U64" s="68"/>
+      <c r="V64" s="68"/>
       <c r="W64" s="45"/>
       <c r="X64" s="45"/>
       <c r="Y64" s="45"/>
-      <c r="Z64" s="88"/>
-      <c r="AA64" s="88"/>
-      <c r="AB64" s="88"/>
+      <c r="Z64" s="68"/>
+      <c r="AA64" s="68"/>
+      <c r="AB64" s="68"/>
       <c r="AC64" s="45"/>
       <c r="AD64" s="45"/>
       <c r="AE64" s="45"/>
-      <c r="AF64" s="88"/>
-      <c r="AG64" s="88"/>
-      <c r="AH64" s="88"/>
+      <c r="AF64" s="68"/>
+      <c r="AG64" s="68"/>
+      <c r="AH64" s="68"/>
       <c r="AI64" s="45"/>
       <c r="AJ64" s="45"/>
       <c r="AK64" s="45"/>
@@ -42777,29 +42777,29 @@
       <c r="K65" s="45"/>
       <c r="L65" s="45"/>
       <c r="M65" s="45"/>
-      <c r="N65" s="88"/>
-      <c r="O65" s="88"/>
-      <c r="P65" s="88"/>
+      <c r="N65" s="68"/>
+      <c r="O65" s="68"/>
+      <c r="P65" s="68"/>
       <c r="Q65" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R65" s="45"/>
       <c r="S65" s="45"/>
-      <c r="T65" s="88"/>
-      <c r="U65" s="88"/>
-      <c r="V65" s="88"/>
+      <c r="T65" s="68"/>
+      <c r="U65" s="68"/>
+      <c r="V65" s="68"/>
       <c r="W65" s="45"/>
       <c r="X65" s="45"/>
       <c r="Y65" s="45"/>
-      <c r="Z65" s="88"/>
-      <c r="AA65" s="88"/>
-      <c r="AB65" s="88"/>
+      <c r="Z65" s="68"/>
+      <c r="AA65" s="68"/>
+      <c r="AB65" s="68"/>
       <c r="AC65" s="45"/>
       <c r="AD65" s="45"/>
       <c r="AE65" s="45"/>
-      <c r="AF65" s="88"/>
-      <c r="AG65" s="88"/>
-      <c r="AH65" s="88"/>
+      <c r="AF65" s="68"/>
+      <c r="AG65" s="68"/>
+      <c r="AH65" s="68"/>
       <c r="AI65" s="45"/>
       <c r="AJ65" s="45"/>
       <c r="AK65" s="45"/>
@@ -42838,29 +42838,29 @@
       <c r="K66" s="45"/>
       <c r="L66" s="45"/>
       <c r="M66" s="45"/>
-      <c r="N66" s="88"/>
-      <c r="O66" s="88"/>
-      <c r="P66" s="88"/>
+      <c r="N66" s="68"/>
+      <c r="O66" s="68"/>
+      <c r="P66" s="68"/>
       <c r="Q66" s="45" t="s">
         <v>156</v>
       </c>
       <c r="R66" s="45"/>
       <c r="S66" s="45"/>
-      <c r="T66" s="88"/>
-      <c r="U66" s="88"/>
-      <c r="V66" s="88"/>
+      <c r="T66" s="68"/>
+      <c r="U66" s="68"/>
+      <c r="V66" s="68"/>
       <c r="W66" s="45"/>
       <c r="X66" s="45"/>
       <c r="Y66" s="45"/>
-      <c r="Z66" s="88"/>
-      <c r="AA66" s="88"/>
-      <c r="AB66" s="88"/>
+      <c r="Z66" s="68"/>
+      <c r="AA66" s="68"/>
+      <c r="AB66" s="68"/>
       <c r="AC66" s="45"/>
       <c r="AD66" s="45"/>
       <c r="AE66" s="45"/>
-      <c r="AF66" s="88"/>
-      <c r="AG66" s="88"/>
-      <c r="AH66" s="88"/>
+      <c r="AF66" s="68"/>
+      <c r="AG66" s="68"/>
+      <c r="AH66" s="68"/>
       <c r="AI66" s="45"/>
       <c r="AJ66" s="45"/>
       <c r="AK66" s="45"/>
@@ -42901,29 +42901,29 @@
       <c r="K67" s="45"/>
       <c r="L67" s="45"/>
       <c r="M67" s="45"/>
-      <c r="N67" s="88"/>
-      <c r="O67" s="88"/>
-      <c r="P67" s="88"/>
+      <c r="N67" s="68"/>
+      <c r="O67" s="68"/>
+      <c r="P67" s="68"/>
       <c r="Q67" s="45" t="s">
         <v>156</v>
       </c>
       <c r="R67" s="45"/>
       <c r="S67" s="45"/>
-      <c r="T67" s="88"/>
-      <c r="U67" s="88"/>
-      <c r="V67" s="88"/>
+      <c r="T67" s="68"/>
+      <c r="U67" s="68"/>
+      <c r="V67" s="68"/>
       <c r="W67" s="45"/>
       <c r="X67" s="45"/>
       <c r="Y67" s="45"/>
-      <c r="Z67" s="88"/>
-      <c r="AA67" s="88"/>
-      <c r="AB67" s="88"/>
+      <c r="Z67" s="68"/>
+      <c r="AA67" s="68"/>
+      <c r="AB67" s="68"/>
       <c r="AC67" s="45"/>
       <c r="AD67" s="45"/>
       <c r="AE67" s="45"/>
-      <c r="AF67" s="88"/>
-      <c r="AG67" s="88"/>
-      <c r="AH67" s="88"/>
+      <c r="AF67" s="68"/>
+      <c r="AG67" s="68"/>
+      <c r="AH67" s="68"/>
       <c r="AI67" s="45"/>
       <c r="AJ67" s="45"/>
       <c r="AK67" s="45"/>
@@ -42962,29 +42962,29 @@
       <c r="K68" s="45"/>
       <c r="L68" s="45"/>
       <c r="M68" s="45"/>
-      <c r="N68" s="88"/>
-      <c r="O68" s="88"/>
-      <c r="P68" s="88"/>
+      <c r="N68" s="68"/>
+      <c r="O68" s="68"/>
+      <c r="P68" s="68"/>
       <c r="Q68" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R68" s="45"/>
       <c r="S68" s="45"/>
-      <c r="T68" s="88"/>
-      <c r="U68" s="88"/>
-      <c r="V68" s="88"/>
+      <c r="T68" s="68"/>
+      <c r="U68" s="68"/>
+      <c r="V68" s="68"/>
       <c r="W68" s="45"/>
       <c r="X68" s="45"/>
       <c r="Y68" s="45"/>
-      <c r="Z68" s="88"/>
-      <c r="AA68" s="88"/>
-      <c r="AB68" s="88"/>
+      <c r="Z68" s="68"/>
+      <c r="AA68" s="68"/>
+      <c r="AB68" s="68"/>
       <c r="AC68" s="45"/>
       <c r="AD68" s="45"/>
       <c r="AE68" s="45"/>
-      <c r="AF68" s="88"/>
-      <c r="AG68" s="88"/>
-      <c r="AH68" s="88"/>
+      <c r="AF68" s="68"/>
+      <c r="AG68" s="68"/>
+      <c r="AH68" s="68"/>
       <c r="AI68" s="45"/>
       <c r="AJ68" s="45"/>
       <c r="AK68" s="45"/>
@@ -43023,29 +43023,29 @@
       <c r="K69" s="45"/>
       <c r="L69" s="45"/>
       <c r="M69" s="45"/>
-      <c r="N69" s="88"/>
-      <c r="O69" s="88"/>
-      <c r="P69" s="88"/>
+      <c r="N69" s="68"/>
+      <c r="O69" s="68"/>
+      <c r="P69" s="68"/>
       <c r="Q69" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R69" s="45"/>
       <c r="S69" s="45"/>
-      <c r="T69" s="88"/>
-      <c r="U69" s="88"/>
-      <c r="V69" s="88"/>
+      <c r="T69" s="68"/>
+      <c r="U69" s="68"/>
+      <c r="V69" s="68"/>
       <c r="W69" s="45"/>
       <c r="X69" s="45"/>
       <c r="Y69" s="45"/>
-      <c r="Z69" s="88"/>
-      <c r="AA69" s="88"/>
-      <c r="AB69" s="88"/>
+      <c r="Z69" s="68"/>
+      <c r="AA69" s="68"/>
+      <c r="AB69" s="68"/>
       <c r="AC69" s="45"/>
       <c r="AD69" s="45"/>
       <c r="AE69" s="45"/>
-      <c r="AF69" s="88"/>
-      <c r="AG69" s="88"/>
-      <c r="AH69" s="88"/>
+      <c r="AF69" s="68"/>
+      <c r="AG69" s="68"/>
+      <c r="AH69" s="68"/>
       <c r="AI69" s="45"/>
       <c r="AJ69" s="45"/>
       <c r="AK69" s="45"/>
@@ -43086,29 +43086,29 @@
       <c r="K70" s="45"/>
       <c r="L70" s="45"/>
       <c r="M70" s="45"/>
-      <c r="N70" s="88"/>
-      <c r="O70" s="88"/>
-      <c r="P70" s="88"/>
+      <c r="N70" s="68"/>
+      <c r="O70" s="68"/>
+      <c r="P70" s="68"/>
       <c r="Q70" s="45" t="s">
         <v>163</v>
       </c>
       <c r="R70" s="45"/>
       <c r="S70" s="45"/>
-      <c r="T70" s="88"/>
-      <c r="U70" s="88"/>
-      <c r="V70" s="88"/>
+      <c r="T70" s="68"/>
+      <c r="U70" s="68"/>
+      <c r="V70" s="68"/>
       <c r="W70" s="45"/>
       <c r="X70" s="45"/>
       <c r="Y70" s="45"/>
-      <c r="Z70" s="88"/>
-      <c r="AA70" s="88"/>
-      <c r="AB70" s="88"/>
+      <c r="Z70" s="68"/>
+      <c r="AA70" s="68"/>
+      <c r="AB70" s="68"/>
       <c r="AC70" s="45"/>
       <c r="AD70" s="45"/>
       <c r="AE70" s="45"/>
-      <c r="AF70" s="88"/>
-      <c r="AG70" s="88"/>
-      <c r="AH70" s="88"/>
+      <c r="AF70" s="68"/>
+      <c r="AG70" s="68"/>
+      <c r="AH70" s="68"/>
       <c r="AI70" s="45"/>
       <c r="AJ70" s="45"/>
       <c r="AK70" s="45"/>
@@ -43147,29 +43147,29 @@
       <c r="K71" s="45"/>
       <c r="L71" s="45"/>
       <c r="M71" s="45"/>
-      <c r="N71" s="88"/>
-      <c r="O71" s="88"/>
-      <c r="P71" s="88"/>
+      <c r="N71" s="68"/>
+      <c r="O71" s="68"/>
+      <c r="P71" s="68"/>
       <c r="Q71" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R71" s="45"/>
       <c r="S71" s="45"/>
-      <c r="T71" s="88"/>
-      <c r="U71" s="88"/>
-      <c r="V71" s="88"/>
+      <c r="T71" s="68"/>
+      <c r="U71" s="68"/>
+      <c r="V71" s="68"/>
       <c r="W71" s="45"/>
       <c r="X71" s="45"/>
       <c r="Y71" s="45"/>
-      <c r="Z71" s="88"/>
-      <c r="AA71" s="88"/>
-      <c r="AB71" s="88"/>
+      <c r="Z71" s="68"/>
+      <c r="AA71" s="68"/>
+      <c r="AB71" s="68"/>
       <c r="AC71" s="45"/>
       <c r="AD71" s="45"/>
       <c r="AE71" s="45"/>
-      <c r="AF71" s="88"/>
-      <c r="AG71" s="88"/>
-      <c r="AH71" s="88"/>
+      <c r="AF71" s="68"/>
+      <c r="AG71" s="68"/>
+      <c r="AH71" s="68"/>
       <c r="AI71" s="45"/>
       <c r="AJ71" s="45"/>
       <c r="AK71" s="45"/>
@@ -43208,29 +43208,29 @@
       <c r="K72" s="45"/>
       <c r="L72" s="45"/>
       <c r="M72" s="45"/>
-      <c r="N72" s="88"/>
-      <c r="O72" s="88"/>
-      <c r="P72" s="88"/>
+      <c r="N72" s="68"/>
+      <c r="O72" s="68"/>
+      <c r="P72" s="68"/>
       <c r="Q72" s="45" t="s">
         <v>159</v>
       </c>
       <c r="R72" s="45"/>
       <c r="S72" s="45"/>
-      <c r="T72" s="88"/>
-      <c r="U72" s="88"/>
-      <c r="V72" s="88"/>
+      <c r="T72" s="68"/>
+      <c r="U72" s="68"/>
+      <c r="V72" s="68"/>
       <c r="W72" s="45"/>
       <c r="X72" s="45"/>
       <c r="Y72" s="45"/>
-      <c r="Z72" s="88"/>
-      <c r="AA72" s="88"/>
-      <c r="AB72" s="88"/>
+      <c r="Z72" s="68"/>
+      <c r="AA72" s="68"/>
+      <c r="AB72" s="68"/>
       <c r="AC72" s="45"/>
       <c r="AD72" s="45"/>
       <c r="AE72" s="45"/>
-      <c r="AF72" s="88"/>
-      <c r="AG72" s="88"/>
-      <c r="AH72" s="88"/>
+      <c r="AF72" s="68"/>
+      <c r="AG72" s="68"/>
+      <c r="AH72" s="68"/>
       <c r="AI72" s="45"/>
       <c r="AJ72" s="45"/>
       <c r="AK72" s="45"/>
@@ -43269,29 +43269,29 @@
       <c r="K73" s="45"/>
       <c r="L73" s="45"/>
       <c r="M73" s="45"/>
-      <c r="N73" s="88"/>
-      <c r="O73" s="88"/>
-      <c r="P73" s="88"/>
+      <c r="N73" s="68"/>
+      <c r="O73" s="68"/>
+      <c r="P73" s="68"/>
       <c r="Q73" s="45" t="s">
         <v>159</v>
       </c>
       <c r="R73" s="45"/>
       <c r="S73" s="45"/>
-      <c r="T73" s="88"/>
-      <c r="U73" s="88"/>
-      <c r="V73" s="88"/>
+      <c r="T73" s="68"/>
+      <c r="U73" s="68"/>
+      <c r="V73" s="68"/>
       <c r="W73" s="45"/>
       <c r="X73" s="45"/>
       <c r="Y73" s="45"/>
-      <c r="Z73" s="88"/>
-      <c r="AA73" s="88"/>
-      <c r="AB73" s="88"/>
+      <c r="Z73" s="68"/>
+      <c r="AA73" s="68"/>
+      <c r="AB73" s="68"/>
       <c r="AC73" s="45"/>
       <c r="AD73" s="45"/>
       <c r="AE73" s="45"/>
-      <c r="AF73" s="88"/>
-      <c r="AG73" s="88"/>
-      <c r="AH73" s="88"/>
+      <c r="AF73" s="68"/>
+      <c r="AG73" s="68"/>
+      <c r="AH73" s="68"/>
       <c r="AI73" s="45"/>
       <c r="AJ73" s="45"/>
       <c r="AK73" s="45"/>
@@ -43330,29 +43330,29 @@
       <c r="K74" s="45"/>
       <c r="L74" s="45"/>
       <c r="M74" s="45"/>
-      <c r="N74" s="88"/>
-      <c r="O74" s="88"/>
-      <c r="P74" s="88"/>
+      <c r="N74" s="68"/>
+      <c r="O74" s="68"/>
+      <c r="P74" s="68"/>
       <c r="Q74" s="45" t="s">
         <v>108</v>
       </c>
       <c r="R74" s="45"/>
       <c r="S74" s="45"/>
-      <c r="T74" s="88"/>
-      <c r="U74" s="88"/>
-      <c r="V74" s="88"/>
+      <c r="T74" s="68"/>
+      <c r="U74" s="68"/>
+      <c r="V74" s="68"/>
       <c r="W74" s="45"/>
       <c r="X74" s="45"/>
       <c r="Y74" s="45"/>
-      <c r="Z74" s="88"/>
-      <c r="AA74" s="88"/>
-      <c r="AB74" s="88"/>
+      <c r="Z74" s="68"/>
+      <c r="AA74" s="68"/>
+      <c r="AB74" s="68"/>
       <c r="AC74" s="45"/>
       <c r="AD74" s="45"/>
       <c r="AE74" s="45"/>
-      <c r="AF74" s="88"/>
-      <c r="AG74" s="88"/>
-      <c r="AH74" s="88"/>
+      <c r="AF74" s="68"/>
+      <c r="AG74" s="68"/>
+      <c r="AH74" s="68"/>
       <c r="AI74" s="45"/>
       <c r="AJ74" s="45"/>
       <c r="AK74" s="45"/>
@@ -43836,6 +43836,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -43848,12 +43854,6 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>